<commit_message>
Japanese has been edited.
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCV-DELL0010\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D90862-005C-4E6C-8D0E-A4E366DE3DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9478BB49-6EDC-4C1F-AB0F-66FAE885DC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1110" windowWidth="28800" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="1470" windowWidth="28800" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -25355,9 +25355,6 @@
     <t>天気予報のソースとして使用されるオンラインサービス。</t>
   </si>
   <si>
-    <t>に</t>
-  </si>
-  <si>
     <t>このアプリケーションをリロードしますか？</t>
   </si>
   <si>
@@ -26382,7 +26379,7 @@
   </si>
   <si>
     <t>Remember login</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>Japanese</t>
@@ -26833,18 +26830,30 @@
   </si>
   <si>
     <t>下のボタンを使用して、Androidのさまざまな管理モードを有効または無効にできます。&lt;br&gt;この機能は慎重に操作してください、デバイスが完全にロックされる可能性があります！&lt;br&gt; Androidで許可する前に、デバイスの所有者とデバイスの管理者を無効にする必要がありますこのアプリケーションをアンインストールします。</t>
+  </si>
+  <si>
+    <t>から</t>
+    <phoneticPr fontId="7"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -26911,6 +26920,9 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -26920,19 +26932,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+  </cellStyleXfs>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -27256,10 +27268,10 @@
   <dimension ref="A1:M714"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2:M714"/>
+      <selection pane="bottomRight" activeCell="M291" sqref="M291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -27310,7 +27322,7 @@
         <v>6484</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>8784</v>
+        <v>8783</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -27351,7 +27363,7 @@
         <v>6485</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>8784</v>
+        <v>8783</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -27474,7 +27486,7 @@
         <v>6488</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>8806</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -27556,7 +27568,7 @@
         <v>6489</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>8807</v>
+        <v>8806</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -27761,7 +27773,7 @@
         <v>6493</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>8799</v>
+        <v>8798</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -28130,7 +28142,7 @@
         <v>6500</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>8785</v>
+        <v>8784</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
@@ -28171,7 +28183,7 @@
         <v>6501</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>8808</v>
+        <v>8807</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
@@ -28786,7 +28798,7 @@
         <v>6514</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>8906</v>
+        <v>8905</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
@@ -29442,7 +29454,7 @@
         <v>6530</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>8907</v>
+        <v>8906</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
@@ -29729,7 +29741,7 @@
         <v>6537</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>8809</v>
+        <v>8808</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
@@ -30344,7 +30356,7 @@
         <v>6551</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>8810</v>
+        <v>8809</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.4">
@@ -30426,7 +30438,7 @@
         <v>7850</v>
       </c>
       <c r="M77" s="5" t="s">
-        <v>8811</v>
+        <v>8810</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
@@ -30795,7 +30807,7 @@
         <v>6559</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>8812</v>
+        <v>8811</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.4">
@@ -30918,7 +30930,7 @@
         <v>6562</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>8908</v>
+        <v>8907</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.4">
@@ -31410,7 +31422,7 @@
         <v>6572</v>
       </c>
       <c r="M101" s="5" t="s">
-        <v>8813</v>
+        <v>8812</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.4">
@@ -33009,7 +33021,7 @@
         <v>6604</v>
       </c>
       <c r="M140" s="5" t="s">
-        <v>8909</v>
+        <v>8908</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.4">
@@ -33173,7 +33185,7 @@
         <v>6608</v>
       </c>
       <c r="M144" s="5" t="s">
-        <v>8910</v>
+        <v>8909</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.4">
@@ -33214,7 +33226,7 @@
         <v>6609</v>
       </c>
       <c r="M145" s="5" t="s">
-        <v>8911</v>
+        <v>8910</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.4">
@@ -33337,7 +33349,7 @@
         <v>6612</v>
       </c>
       <c r="M148" s="5" t="s">
-        <v>8814</v>
+        <v>8813</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.4">
@@ -33378,7 +33390,7 @@
         <v>6613</v>
       </c>
       <c r="M149" s="5" t="s">
-        <v>8815</v>
+        <v>8814</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.4">
@@ -33460,7 +33472,7 @@
         <v>6615</v>
       </c>
       <c r="M151" s="5" t="s">
-        <v>8816</v>
+        <v>8815</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.4">
@@ -33501,7 +33513,7 @@
         <v>6616</v>
       </c>
       <c r="M152" s="5" t="s">
-        <v>8817</v>
+        <v>8816</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.4">
@@ -33788,7 +33800,7 @@
         <v>6623</v>
       </c>
       <c r="M159" s="5" t="s">
-        <v>8818</v>
+        <v>8817</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.4">
@@ -33993,7 +34005,7 @@
         <v>6628</v>
       </c>
       <c r="M164" s="5" t="s">
-        <v>8912</v>
+        <v>8911</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.4">
@@ -34116,7 +34128,7 @@
         <v>6631</v>
       </c>
       <c r="M167" s="5" t="s">
-        <v>8819</v>
+        <v>8818</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.4">
@@ -34444,7 +34456,7 @@
         <v>6637</v>
       </c>
       <c r="M175" s="5" t="s">
-        <v>8820</v>
+        <v>8819</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.4">
@@ -34567,7 +34579,7 @@
         <v>6640</v>
       </c>
       <c r="M178" s="5" t="s">
-        <v>8821</v>
+        <v>8820</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.4">
@@ -34731,7 +34743,7 @@
         <v>5409</v>
       </c>
       <c r="M182" s="5" t="s">
-        <v>8822</v>
+        <v>8821</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.4">
@@ -34854,7 +34866,7 @@
         <v>6646</v>
       </c>
       <c r="M185" s="5" t="s">
-        <v>8823</v>
+        <v>8822</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.4">
@@ -34895,7 +34907,7 @@
         <v>6647</v>
       </c>
       <c r="M186" s="5" t="s">
-        <v>8824</v>
+        <v>8823</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.4">
@@ -34936,7 +34948,7 @@
         <v>6648</v>
       </c>
       <c r="M187" s="5" t="s">
-        <v>8825</v>
+        <v>8824</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.4">
@@ -34977,7 +34989,7 @@
         <v>6649</v>
       </c>
       <c r="M188" s="5" t="s">
-        <v>8826</v>
+        <v>8825</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.4">
@@ -35100,7 +35112,7 @@
         <v>6652</v>
       </c>
       <c r="M191" s="5" t="s">
-        <v>8827</v>
+        <v>8826</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.4">
@@ -35141,7 +35153,7 @@
         <v>6653</v>
       </c>
       <c r="M192" s="5" t="s">
-        <v>8828</v>
+        <v>8827</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.4">
@@ -35264,7 +35276,7 @@
         <v>6656</v>
       </c>
       <c r="M195" s="5" t="s">
-        <v>8829</v>
+        <v>8828</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.4">
@@ -35305,7 +35317,7 @@
         <v>6657</v>
       </c>
       <c r="M196" s="5" t="s">
-        <v>8830</v>
+        <v>8829</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.4">
@@ -35387,7 +35399,7 @@
         <v>6659</v>
       </c>
       <c r="M198" s="5" t="s">
-        <v>8831</v>
+        <v>8830</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.4">
@@ -35428,7 +35440,7 @@
         <v>6660</v>
       </c>
       <c r="M199" s="5" t="s">
-        <v>8832</v>
+        <v>8831</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.4">
@@ -35469,7 +35481,7 @@
         <v>6661</v>
       </c>
       <c r="M200" s="5" t="s">
-        <v>8833</v>
+        <v>8832</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.4">
@@ -35551,7 +35563,7 @@
         <v>6663</v>
       </c>
       <c r="M202" s="5" t="s">
-        <v>8834</v>
+        <v>8833</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.4">
@@ -35674,7 +35686,7 @@
         <v>8099</v>
       </c>
       <c r="M205" s="5" t="s">
-        <v>8835</v>
+        <v>8834</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.4">
@@ -35715,7 +35727,7 @@
         <v>6666</v>
       </c>
       <c r="M206" s="5" t="s">
-        <v>8836</v>
+        <v>8835</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.4">
@@ -35756,7 +35768,7 @@
         <v>6667</v>
       </c>
       <c r="M207" s="5" t="s">
-        <v>8837</v>
+        <v>8836</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.4">
@@ -35920,7 +35932,7 @@
         <v>6671</v>
       </c>
       <c r="M211" s="5" t="s">
-        <v>8838</v>
+        <v>8837</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.4">
@@ -35961,7 +35973,7 @@
         <v>6672</v>
       </c>
       <c r="M212" s="5" t="s">
-        <v>8839</v>
+        <v>8838</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.4">
@@ -36207,7 +36219,7 @@
         <v>6678</v>
       </c>
       <c r="M218" s="5" t="s">
-        <v>8840</v>
+        <v>8839</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.4">
@@ -36248,7 +36260,7 @@
         <v>6679</v>
       </c>
       <c r="M219" s="5" t="s">
-        <v>8841</v>
+        <v>8840</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.4">
@@ -36576,7 +36588,7 @@
         <v>6687</v>
       </c>
       <c r="M227" s="5" t="s">
-        <v>8842</v>
+        <v>8841</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.4">
@@ -36617,7 +36629,7 @@
         <v>6688</v>
       </c>
       <c r="M228" s="5" t="s">
-        <v>8843</v>
+        <v>8842</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.4">
@@ -36658,7 +36670,7 @@
         <v>6689</v>
       </c>
       <c r="M229" s="5" t="s">
-        <v>8844</v>
+        <v>8843</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.4">
@@ -36699,7 +36711,7 @@
         <v>6690</v>
       </c>
       <c r="M230" s="5" t="s">
-        <v>8845</v>
+        <v>8844</v>
       </c>
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.4">
@@ -36740,7 +36752,7 @@
         <v>6691</v>
       </c>
       <c r="M231" s="5" t="s">
-        <v>8846</v>
+        <v>8845</v>
       </c>
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.4">
@@ -36904,7 +36916,7 @@
         <v>6694</v>
       </c>
       <c r="M235" s="5" t="s">
-        <v>8847</v>
+        <v>8846</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.4">
@@ -36986,7 +36998,7 @@
         <v>6696</v>
       </c>
       <c r="M237" s="5" t="s">
-        <v>8848</v>
+        <v>8847</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.4">
@@ -37027,7 +37039,7 @@
         <v>6697</v>
       </c>
       <c r="M238" s="5" t="s">
-        <v>8849</v>
+        <v>8848</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.4">
@@ -37068,7 +37080,7 @@
         <v>6698</v>
       </c>
       <c r="M239" s="5" t="s">
-        <v>8850</v>
+        <v>8849</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.4">
@@ -37109,7 +37121,7 @@
         <v>6699</v>
       </c>
       <c r="M240" s="5" t="s">
-        <v>8851</v>
+        <v>8850</v>
       </c>
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.4">
@@ -37273,7 +37285,7 @@
         <v>6703</v>
       </c>
       <c r="M244" s="5" t="s">
-        <v>8852</v>
+        <v>8851</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.4">
@@ -37519,7 +37531,7 @@
         <v>6709</v>
       </c>
       <c r="M250" s="5" t="s">
-        <v>8853</v>
+        <v>8852</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.4">
@@ -37642,7 +37654,7 @@
         <v>6712</v>
       </c>
       <c r="M253" s="5" t="s">
-        <v>8854</v>
+        <v>8853</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.4">
@@ -37683,7 +37695,7 @@
         <v>6713</v>
       </c>
       <c r="M254" s="5" t="s">
-        <v>8855</v>
+        <v>8854</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.4">
@@ -37765,7 +37777,7 @@
         <v>6715</v>
       </c>
       <c r="M256" s="5" t="s">
-        <v>8856</v>
+        <v>8855</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.4">
@@ -37806,7 +37818,7 @@
         <v>6716</v>
       </c>
       <c r="M257" s="5" t="s">
-        <v>8857</v>
+        <v>8856</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.4">
@@ -37929,7 +37941,7 @@
         <v>6719</v>
       </c>
       <c r="M260" s="5" t="s">
-        <v>8858</v>
+        <v>8857</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.4">
@@ -37970,7 +37982,7 @@
         <v>6720</v>
       </c>
       <c r="M261" s="5" t="s">
-        <v>8859</v>
+        <v>8858</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.4">
@@ -38011,7 +38023,7 @@
         <v>6721</v>
       </c>
       <c r="M262" s="5" t="s">
-        <v>8860</v>
+        <v>8859</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.4">
@@ -38052,7 +38064,7 @@
         <v>6722</v>
       </c>
       <c r="M263" s="5" t="s">
-        <v>8861</v>
+        <v>8860</v>
       </c>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.4">
@@ -38175,7 +38187,7 @@
         <v>6725</v>
       </c>
       <c r="M266" s="5" t="s">
-        <v>8862</v>
+        <v>8861</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.4">
@@ -38298,7 +38310,7 @@
         <v>6728</v>
       </c>
       <c r="M269" s="5" t="s">
-        <v>8863</v>
+        <v>8862</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.4">
@@ -38339,7 +38351,7 @@
         <v>6729</v>
       </c>
       <c r="M270" s="5" t="s">
-        <v>8864</v>
+        <v>8863</v>
       </c>
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.4">
@@ -38462,7 +38474,7 @@
         <v>6731</v>
       </c>
       <c r="M273" s="5" t="s">
-        <v>8865</v>
+        <v>8864</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.4">
@@ -38544,7 +38556,7 @@
         <v>6733</v>
       </c>
       <c r="M275" s="5" t="s">
-        <v>8866</v>
+        <v>8865</v>
       </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.4">
@@ -38585,7 +38597,7 @@
         <v>6734</v>
       </c>
       <c r="M276" s="5" t="s">
-        <v>8867</v>
+        <v>8866</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.4">
@@ -38626,7 +38638,7 @@
         <v>6735</v>
       </c>
       <c r="M277" s="5" t="s">
-        <v>8868</v>
+        <v>8867</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.4">
@@ -38667,7 +38679,7 @@
         <v>6736</v>
       </c>
       <c r="M278" s="5" t="s">
-        <v>8869</v>
+        <v>8868</v>
       </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.4">
@@ -38790,7 +38802,7 @@
         <v>6739</v>
       </c>
       <c r="M281" s="5" t="s">
-        <v>8870</v>
+        <v>8869</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.4">
@@ -38831,7 +38843,7 @@
         <v>6740</v>
       </c>
       <c r="M282" s="5" t="s">
-        <v>8871</v>
+        <v>8870</v>
       </c>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.4">
@@ -39036,7 +39048,7 @@
         <v>6744</v>
       </c>
       <c r="M287" s="5" t="s">
-        <v>8913</v>
+        <v>8912</v>
       </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.4">
@@ -39199,8 +39211,8 @@
       <c r="L291" t="s">
         <v>5514</v>
       </c>
-      <c r="M291" s="5" t="s">
-        <v>8441</v>
+      <c r="M291" s="6" t="s">
+        <v>8933</v>
       </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.4">
@@ -39241,7 +39253,7 @@
         <v>6747</v>
       </c>
       <c r="M292" s="5" t="s">
-        <v>8442</v>
+        <v>8441</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.4">
@@ -39282,7 +39294,7 @@
         <v>6748</v>
       </c>
       <c r="M293" s="5" t="s">
-        <v>8872</v>
+        <v>8871</v>
       </c>
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.4">
@@ -39323,7 +39335,7 @@
         <v>6749</v>
       </c>
       <c r="M294" s="5" t="s">
-        <v>8443</v>
+        <v>8442</v>
       </c>
     </row>
     <row r="295" spans="1:13" x14ac:dyDescent="0.4">
@@ -39364,7 +39376,7 @@
         <v>6750</v>
       </c>
       <c r="M295" s="5" t="s">
-        <v>8444</v>
+        <v>8443</v>
       </c>
     </row>
     <row r="296" spans="1:13" x14ac:dyDescent="0.4">
@@ -39405,7 +39417,7 @@
         <v>6751</v>
       </c>
       <c r="M296" s="5" t="s">
-        <v>8445</v>
+        <v>8444</v>
       </c>
     </row>
     <row r="297" spans="1:13" x14ac:dyDescent="0.4">
@@ -39446,7 +39458,7 @@
         <v>6752</v>
       </c>
       <c r="M297" s="5" t="s">
-        <v>8446</v>
+        <v>8445</v>
       </c>
     </row>
     <row r="298" spans="1:13" x14ac:dyDescent="0.4">
@@ -39487,7 +39499,7 @@
         <v>6753</v>
       </c>
       <c r="M298" s="5" t="s">
-        <v>8446</v>
+        <v>8445</v>
       </c>
     </row>
     <row r="299" spans="1:13" x14ac:dyDescent="0.4">
@@ -39528,7 +39540,7 @@
         <v>6754</v>
       </c>
       <c r="M299" s="5" t="s">
-        <v>8447</v>
+        <v>8446</v>
       </c>
     </row>
     <row r="300" spans="1:13" x14ac:dyDescent="0.4">
@@ -39569,7 +39581,7 @@
         <v>6755</v>
       </c>
       <c r="M300" s="5" t="s">
-        <v>8448</v>
+        <v>8447</v>
       </c>
     </row>
     <row r="301" spans="1:13" x14ac:dyDescent="0.4">
@@ -39610,7 +39622,7 @@
         <v>6756</v>
       </c>
       <c r="M301" s="5" t="s">
-        <v>8449</v>
+        <v>8448</v>
       </c>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.4">
@@ -39651,7 +39663,7 @@
         <v>6757</v>
       </c>
       <c r="M302" s="5" t="s">
-        <v>8450</v>
+        <v>8449</v>
       </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.4">
@@ -39692,7 +39704,7 @@
         <v>6758</v>
       </c>
       <c r="M303" s="5" t="s">
-        <v>8451</v>
+        <v>8450</v>
       </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.4">
@@ -39733,7 +39745,7 @@
         <v>6759</v>
       </c>
       <c r="M304" s="5" t="s">
-        <v>8452</v>
+        <v>8451</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.4">
@@ -39774,7 +39786,7 @@
         <v>6760</v>
       </c>
       <c r="M305" s="5" t="s">
-        <v>8453</v>
+        <v>8452</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.4">
@@ -39815,7 +39827,7 @@
         <v>6761</v>
       </c>
       <c r="M306" s="5" t="s">
-        <v>8454</v>
+        <v>8453</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.4">
@@ -39856,7 +39868,7 @@
         <v>6762</v>
       </c>
       <c r="M307" s="5" t="s">
-        <v>8873</v>
+        <v>8872</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.4">
@@ -39897,7 +39909,7 @@
         <v>6763</v>
       </c>
       <c r="M308" s="5" t="s">
-        <v>8455</v>
+        <v>8454</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.4">
@@ -39938,7 +39950,7 @@
         <v>6764</v>
       </c>
       <c r="M309" s="5" t="s">
-        <v>8456</v>
+        <v>8455</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.4">
@@ -39979,7 +39991,7 @@
         <v>6765</v>
       </c>
       <c r="M310" s="5" t="s">
-        <v>8457</v>
+        <v>8456</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.4">
@@ -40020,7 +40032,7 @@
         <v>6766</v>
       </c>
       <c r="M311" s="5" t="s">
-        <v>8458</v>
+        <v>8457</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.4">
@@ -40061,7 +40073,7 @@
         <v>6767</v>
       </c>
       <c r="M312" s="5" t="s">
-        <v>8459</v>
+        <v>8458</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.4">
@@ -40102,7 +40114,7 @@
         <v>6768</v>
       </c>
       <c r="M313" s="5" t="s">
-        <v>8460</v>
+        <v>8459</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.4">
@@ -40143,7 +40155,7 @@
         <v>5537</v>
       </c>
       <c r="M314" s="5" t="s">
-        <v>8461</v>
+        <v>8460</v>
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.4">
@@ -40184,7 +40196,7 @@
         <v>6769</v>
       </c>
       <c r="M315" s="5" t="s">
-        <v>8462</v>
+        <v>8461</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.4">
@@ -40225,7 +40237,7 @@
         <v>6770</v>
       </c>
       <c r="M316" s="5" t="s">
-        <v>8874</v>
+        <v>8873</v>
       </c>
     </row>
     <row r="317" spans="1:13" x14ac:dyDescent="0.4">
@@ -40266,7 +40278,7 @@
         <v>6771</v>
       </c>
       <c r="M317" s="5" t="s">
-        <v>8463</v>
+        <v>8462</v>
       </c>
     </row>
     <row r="318" spans="1:13" x14ac:dyDescent="0.4">
@@ -40307,7 +40319,7 @@
         <v>6642</v>
       </c>
       <c r="M318" s="5" t="s">
-        <v>8464</v>
+        <v>8463</v>
       </c>
     </row>
     <row r="319" spans="1:13" x14ac:dyDescent="0.4">
@@ -40348,7 +40360,7 @@
         <v>6772</v>
       </c>
       <c r="M319" s="5" t="s">
-        <v>8465</v>
+        <v>8464</v>
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.4">
@@ -40389,7 +40401,7 @@
         <v>6773</v>
       </c>
       <c r="M320" s="5" t="s">
-        <v>8466</v>
+        <v>8465</v>
       </c>
     </row>
     <row r="321" spans="1:13" x14ac:dyDescent="0.4">
@@ -40430,7 +40442,7 @@
         <v>6774</v>
       </c>
       <c r="M321" s="5" t="s">
-        <v>8467</v>
+        <v>8466</v>
       </c>
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.4">
@@ -40471,7 +40483,7 @@
         <v>6775</v>
       </c>
       <c r="M322" s="5" t="s">
-        <v>8468</v>
+        <v>8467</v>
       </c>
     </row>
     <row r="323" spans="1:13" x14ac:dyDescent="0.4">
@@ -40512,7 +40524,7 @@
         <v>6776</v>
       </c>
       <c r="M323" s="5" t="s">
-        <v>8469</v>
+        <v>8468</v>
       </c>
     </row>
     <row r="324" spans="1:13" x14ac:dyDescent="0.4">
@@ -40553,7 +40565,7 @@
         <v>6777</v>
       </c>
       <c r="M324" s="5" t="s">
-        <v>8470</v>
+        <v>8469</v>
       </c>
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.4">
@@ -40594,7 +40606,7 @@
         <v>6778</v>
       </c>
       <c r="M325" s="5" t="s">
-        <v>8471</v>
+        <v>8470</v>
       </c>
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.4">
@@ -40635,7 +40647,7 @@
         <v>6779</v>
       </c>
       <c r="M326" s="5" t="s">
-        <v>8472</v>
+        <v>8471</v>
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.4">
@@ -40676,7 +40688,7 @@
         <v>6780</v>
       </c>
       <c r="M327" s="5" t="s">
-        <v>8473</v>
+        <v>8472</v>
       </c>
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.4">
@@ -40717,7 +40729,7 @@
         <v>6781</v>
       </c>
       <c r="M328" s="5" t="s">
-        <v>8474</v>
+        <v>8473</v>
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.4">
@@ -40758,7 +40770,7 @@
         <v>6782</v>
       </c>
       <c r="M329" s="5" t="s">
-        <v>8475</v>
+        <v>8474</v>
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.4">
@@ -40799,7 +40811,7 @@
         <v>6783</v>
       </c>
       <c r="M330" s="5" t="s">
-        <v>8800</v>
+        <v>8799</v>
       </c>
     </row>
     <row r="331" spans="1:13" x14ac:dyDescent="0.4">
@@ -40840,7 +40852,7 @@
         <v>5553</v>
       </c>
       <c r="M331" s="5" t="s">
-        <v>8476</v>
+        <v>8475</v>
       </c>
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.4">
@@ -40881,7 +40893,7 @@
         <v>6784</v>
       </c>
       <c r="M332" s="5" t="s">
-        <v>8477</v>
+        <v>8476</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.4">
@@ -40922,7 +40934,7 @@
         <v>6785</v>
       </c>
       <c r="M333" s="5" t="s">
-        <v>8478</v>
+        <v>8477</v>
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.4">
@@ -40963,7 +40975,7 @@
         <v>6786</v>
       </c>
       <c r="M334" s="5" t="s">
-        <v>8479</v>
+        <v>8478</v>
       </c>
     </row>
     <row r="335" spans="1:13" x14ac:dyDescent="0.4">
@@ -41004,7 +41016,7 @@
         <v>6787</v>
       </c>
       <c r="M335" s="5" t="s">
-        <v>8480</v>
+        <v>8479</v>
       </c>
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.4">
@@ -41045,7 +41057,7 @@
         <v>6788</v>
       </c>
       <c r="M336" s="5" t="s">
-        <v>8481</v>
+        <v>8480</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.4">
@@ -41086,7 +41098,7 @@
         <v>6789</v>
       </c>
       <c r="M337" s="5" t="s">
-        <v>8482</v>
+        <v>8481</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.4">
@@ -41127,7 +41139,7 @@
         <v>6790</v>
       </c>
       <c r="M338" s="5" t="s">
-        <v>8914</v>
+        <v>8913</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.4">
@@ -41209,7 +41221,7 @@
         <v>6791</v>
       </c>
       <c r="M340" s="5" t="s">
-        <v>8483</v>
+        <v>8482</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.4">
@@ -41250,7 +41262,7 @@
         <v>6792</v>
       </c>
       <c r="M341" s="5" t="s">
-        <v>8484</v>
+        <v>8483</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.4">
@@ -41291,7 +41303,7 @@
         <v>6793</v>
       </c>
       <c r="M342" s="5" t="s">
-        <v>8485</v>
+        <v>8484</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.4">
@@ -41332,7 +41344,7 @@
         <v>6794</v>
       </c>
       <c r="M343" s="5" t="s">
-        <v>8486</v>
+        <v>8485</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.4">
@@ -41373,7 +41385,7 @@
         <v>6795</v>
       </c>
       <c r="M344" s="5" t="s">
-        <v>8487</v>
+        <v>8486</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.4">
@@ -41414,7 +41426,7 @@
         <v>6796</v>
       </c>
       <c r="M345" s="5" t="s">
-        <v>8488</v>
+        <v>8487</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.4">
@@ -41455,7 +41467,7 @@
         <v>6797</v>
       </c>
       <c r="M346" s="5" t="s">
-        <v>8489</v>
+        <v>8488</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.4">
@@ -41496,7 +41508,7 @@
         <v>6798</v>
       </c>
       <c r="M347" s="5" t="s">
-        <v>8490</v>
+        <v>8489</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.4">
@@ -41537,7 +41549,7 @@
         <v>6799</v>
       </c>
       <c r="M348" s="5" t="s">
-        <v>8491</v>
+        <v>8490</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.4">
@@ -41578,7 +41590,7 @@
         <v>6800</v>
       </c>
       <c r="M349" s="5" t="s">
-        <v>8492</v>
+        <v>8491</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.4">
@@ -41619,7 +41631,7 @@
         <v>6801</v>
       </c>
       <c r="M350" s="5" t="s">
-        <v>8493</v>
+        <v>8492</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.4">
@@ -41660,7 +41672,7 @@
         <v>6802</v>
       </c>
       <c r="M351" s="5" t="s">
-        <v>8875</v>
+        <v>8874</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.4">
@@ -41701,7 +41713,7 @@
         <v>6803</v>
       </c>
       <c r="M352" s="5" t="s">
-        <v>8494</v>
+        <v>8493</v>
       </c>
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.4">
@@ -41742,7 +41754,7 @@
         <v>6804</v>
       </c>
       <c r="M353" s="5" t="s">
-        <v>8495</v>
+        <v>8494</v>
       </c>
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.4">
@@ -41783,7 +41795,7 @@
         <v>6805</v>
       </c>
       <c r="M354" s="5" t="s">
-        <v>8496</v>
+        <v>8495</v>
       </c>
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.4">
@@ -41824,7 +41836,7 @@
         <v>6806</v>
       </c>
       <c r="M355" s="5" t="s">
-        <v>8497</v>
+        <v>8496</v>
       </c>
     </row>
     <row r="356" spans="1:13" x14ac:dyDescent="0.4">
@@ -41865,7 +41877,7 @@
         <v>6807</v>
       </c>
       <c r="M356" s="5" t="s">
-        <v>8498</v>
+        <v>8497</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.4">
@@ -41906,7 +41918,7 @@
         <v>6808</v>
       </c>
       <c r="M357" s="5" t="s">
-        <v>8915</v>
+        <v>8914</v>
       </c>
     </row>
     <row r="358" spans="1:13" x14ac:dyDescent="0.4">
@@ -41947,7 +41959,7 @@
         <v>6809</v>
       </c>
       <c r="M358" s="5" t="s">
-        <v>8499</v>
+        <v>8498</v>
       </c>
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.4">
@@ -41988,7 +42000,7 @@
         <v>6810</v>
       </c>
       <c r="M359" s="5" t="s">
-        <v>8500</v>
+        <v>8499</v>
       </c>
     </row>
     <row r="360" spans="1:13" x14ac:dyDescent="0.4">
@@ -42029,7 +42041,7 @@
         <v>6811</v>
       </c>
       <c r="M360" s="5" t="s">
-        <v>8501</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="361" spans="1:13" x14ac:dyDescent="0.4">
@@ -42070,7 +42082,7 @@
         <v>6812</v>
       </c>
       <c r="M361" s="5" t="s">
-        <v>8502</v>
+        <v>8501</v>
       </c>
     </row>
     <row r="362" spans="1:13" x14ac:dyDescent="0.4">
@@ -42111,7 +42123,7 @@
         <v>5584</v>
       </c>
       <c r="M362" s="5" t="s">
-        <v>8503</v>
+        <v>8502</v>
       </c>
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.4">
@@ -42152,7 +42164,7 @@
         <v>6813</v>
       </c>
       <c r="M363" s="5" t="s">
-        <v>8504</v>
+        <v>8503</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.4">
@@ -42193,7 +42205,7 @@
         <v>6811</v>
       </c>
       <c r="M364" s="5" t="s">
-        <v>8501</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.4">
@@ -42234,7 +42246,7 @@
         <v>5586</v>
       </c>
       <c r="M365" s="5" t="s">
-        <v>8505</v>
+        <v>8504</v>
       </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.4">
@@ -42275,7 +42287,7 @@
         <v>6814</v>
       </c>
       <c r="M366" s="5" t="s">
-        <v>8506</v>
+        <v>8505</v>
       </c>
     </row>
     <row r="367" spans="1:13" x14ac:dyDescent="0.4">
@@ -42316,7 +42328,7 @@
         <v>6815</v>
       </c>
       <c r="M367" s="5" t="s">
-        <v>8507</v>
+        <v>8506</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.4">
@@ -42357,7 +42369,7 @@
         <v>6816</v>
       </c>
       <c r="M368" s="5" t="s">
-        <v>8508</v>
+        <v>8507</v>
       </c>
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.4">
@@ -42398,7 +42410,7 @@
         <v>6817</v>
       </c>
       <c r="M369" s="5" t="s">
-        <v>8509</v>
+        <v>8508</v>
       </c>
     </row>
     <row r="370" spans="1:13" x14ac:dyDescent="0.4">
@@ -42439,7 +42451,7 @@
         <v>6818</v>
       </c>
       <c r="M370" s="5" t="s">
-        <v>8510</v>
+        <v>8509</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.4">
@@ -42480,7 +42492,7 @@
         <v>6819</v>
       </c>
       <c r="M371" s="5" t="s">
-        <v>8511</v>
+        <v>8510</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.4">
@@ -42521,7 +42533,7 @@
         <v>6820</v>
       </c>
       <c r="M372" s="5" t="s">
-        <v>8512</v>
+        <v>8511</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.4">
@@ -42562,7 +42574,7 @@
         <v>6821</v>
       </c>
       <c r="M373" s="5" t="s">
-        <v>8513</v>
+        <v>8512</v>
       </c>
     </row>
     <row r="374" spans="1:13" x14ac:dyDescent="0.4">
@@ -42603,7 +42615,7 @@
         <v>6822</v>
       </c>
       <c r="M374" s="5" t="s">
-        <v>8513</v>
+        <v>8512</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.4">
@@ -42644,7 +42656,7 @@
         <v>6823</v>
       </c>
       <c r="M375" s="5" t="s">
-        <v>8514</v>
+        <v>8513</v>
       </c>
     </row>
     <row r="376" spans="1:13" x14ac:dyDescent="0.4">
@@ -42685,7 +42697,7 @@
         <v>6824</v>
       </c>
       <c r="M376" s="5" t="s">
-        <v>8515</v>
+        <v>8514</v>
       </c>
     </row>
     <row r="377" spans="1:13" x14ac:dyDescent="0.4">
@@ -42726,7 +42738,7 @@
         <v>6825</v>
       </c>
       <c r="M377" s="5" t="s">
-        <v>8516</v>
+        <v>8515</v>
       </c>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.4">
@@ -42767,7 +42779,7 @@
         <v>6826</v>
       </c>
       <c r="M378" s="5" t="s">
-        <v>8517</v>
+        <v>8516</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.4">
@@ -42808,7 +42820,7 @@
         <v>6827</v>
       </c>
       <c r="M379" s="5" t="s">
-        <v>8518</v>
+        <v>8517</v>
       </c>
     </row>
     <row r="380" spans="1:13" x14ac:dyDescent="0.4">
@@ -42849,7 +42861,7 @@
         <v>6828</v>
       </c>
       <c r="M380" s="5" t="s">
-        <v>8519</v>
+        <v>8518</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.4">
@@ -42890,7 +42902,7 @@
         <v>6829</v>
       </c>
       <c r="M381" s="5" t="s">
-        <v>8520</v>
+        <v>8519</v>
       </c>
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.4">
@@ -42931,7 +42943,7 @@
         <v>6830</v>
       </c>
       <c r="M382" s="5" t="s">
-        <v>8521</v>
+        <v>8520</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.4">
@@ -42972,7 +42984,7 @@
         <v>6831</v>
       </c>
       <c r="M383" s="5" t="s">
-        <v>8522</v>
+        <v>8521</v>
       </c>
     </row>
     <row r="384" spans="1:13" x14ac:dyDescent="0.4">
@@ -43013,7 +43025,7 @@
         <v>6832</v>
       </c>
       <c r="M384" s="5" t="s">
-        <v>8523</v>
+        <v>8522</v>
       </c>
     </row>
     <row r="385" spans="1:13" x14ac:dyDescent="0.4">
@@ -43054,7 +43066,7 @@
         <v>6833</v>
       </c>
       <c r="M385" s="5" t="s">
-        <v>8524</v>
+        <v>8523</v>
       </c>
     </row>
     <row r="386" spans="1:13" x14ac:dyDescent="0.4">
@@ -43095,7 +43107,7 @@
         <v>6834</v>
       </c>
       <c r="M386" s="5" t="s">
-        <v>8525</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="387" spans="1:13" x14ac:dyDescent="0.4">
@@ -43136,7 +43148,7 @@
         <v>6835</v>
       </c>
       <c r="M387" s="5" t="s">
-        <v>8876</v>
+        <v>8875</v>
       </c>
     </row>
     <row r="388" spans="1:13" x14ac:dyDescent="0.4">
@@ -43177,7 +43189,7 @@
         <v>6836</v>
       </c>
       <c r="M388" s="5" t="s">
-        <v>8526</v>
+        <v>8525</v>
       </c>
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.4">
@@ -43218,7 +43230,7 @@
         <v>6837</v>
       </c>
       <c r="M389" s="5" t="s">
-        <v>8877</v>
+        <v>8876</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.4">
@@ -43259,7 +43271,7 @@
         <v>6838</v>
       </c>
       <c r="M390" s="5" t="s">
-        <v>8878</v>
+        <v>8877</v>
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.4">
@@ -43300,7 +43312,7 @@
         <v>6839</v>
       </c>
       <c r="M391" s="5" t="s">
-        <v>8527</v>
+        <v>8526</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.4">
@@ -43341,7 +43353,7 @@
         <v>6840</v>
       </c>
       <c r="M392" s="5" t="s">
-        <v>8879</v>
+        <v>8878</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.4">
@@ -43382,7 +43394,7 @@
         <v>6841</v>
       </c>
       <c r="M393" s="5" t="s">
-        <v>8528</v>
+        <v>8527</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.4">
@@ -43423,7 +43435,7 @@
         <v>6842</v>
       </c>
       <c r="M394" s="5" t="s">
-        <v>8529</v>
+        <v>8528</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.4">
@@ -43464,7 +43476,7 @@
         <v>6843</v>
       </c>
       <c r="M395" s="5" t="s">
-        <v>8916</v>
+        <v>8915</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.4">
@@ -43505,7 +43517,7 @@
         <v>6844</v>
       </c>
       <c r="M396" s="5" t="s">
-        <v>8530</v>
+        <v>8529</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.4">
@@ -43546,7 +43558,7 @@
         <v>6845</v>
       </c>
       <c r="M397" s="5" t="s">
-        <v>8531</v>
+        <v>8530</v>
       </c>
     </row>
     <row r="398" spans="1:13" x14ac:dyDescent="0.4">
@@ -43587,7 +43599,7 @@
         <v>6846</v>
       </c>
       <c r="M398" s="5" t="s">
-        <v>8532</v>
+        <v>8531</v>
       </c>
     </row>
     <row r="399" spans="1:13" x14ac:dyDescent="0.4">
@@ -43628,7 +43640,7 @@
         <v>6847</v>
       </c>
       <c r="M399" s="5" t="s">
-        <v>8533</v>
+        <v>8532</v>
       </c>
     </row>
     <row r="400" spans="1:13" x14ac:dyDescent="0.4">
@@ -43669,7 +43681,7 @@
         <v>5620</v>
       </c>
       <c r="M400" s="5" t="s">
-        <v>8534</v>
+        <v>8533</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.4">
@@ -43710,7 +43722,7 @@
         <v>6848</v>
       </c>
       <c r="M401" s="5" t="s">
-        <v>8535</v>
+        <v>8534</v>
       </c>
     </row>
     <row r="402" spans="1:13" x14ac:dyDescent="0.4">
@@ -43751,7 +43763,7 @@
         <v>6849</v>
       </c>
       <c r="M402" s="5" t="s">
-        <v>8536</v>
+        <v>8535</v>
       </c>
     </row>
     <row r="403" spans="1:13" x14ac:dyDescent="0.4">
@@ -43792,7 +43804,7 @@
         <v>6850</v>
       </c>
       <c r="M403" s="5" t="s">
-        <v>8537</v>
+        <v>8536</v>
       </c>
     </row>
     <row r="404" spans="1:13" x14ac:dyDescent="0.4">
@@ -43833,7 +43845,7 @@
         <v>6851</v>
       </c>
       <c r="M404" s="5" t="s">
-        <v>8538</v>
+        <v>8537</v>
       </c>
     </row>
     <row r="405" spans="1:13" x14ac:dyDescent="0.4">
@@ -43874,7 +43886,7 @@
         <v>6852</v>
       </c>
       <c r="M405" s="5" t="s">
-        <v>8880</v>
+        <v>8879</v>
       </c>
     </row>
     <row r="406" spans="1:13" x14ac:dyDescent="0.4">
@@ -43915,7 +43927,7 @@
         <v>6853</v>
       </c>
       <c r="M406" s="5" t="s">
-        <v>8539</v>
+        <v>8538</v>
       </c>
     </row>
     <row r="407" spans="1:13" x14ac:dyDescent="0.4">
@@ -43956,7 +43968,7 @@
         <v>6854</v>
       </c>
       <c r="M407" s="5" t="s">
-        <v>8540</v>
+        <v>8539</v>
       </c>
     </row>
     <row r="408" spans="1:13" x14ac:dyDescent="0.4">
@@ -43997,7 +44009,7 @@
         <v>6855</v>
       </c>
       <c r="M408" s="5" t="s">
-        <v>8541</v>
+        <v>8540</v>
       </c>
     </row>
     <row r="409" spans="1:13" x14ac:dyDescent="0.4">
@@ -44038,7 +44050,7 @@
         <v>6856</v>
       </c>
       <c r="M409" s="5" t="s">
-        <v>8542</v>
+        <v>8541</v>
       </c>
     </row>
     <row r="410" spans="1:13" x14ac:dyDescent="0.4">
@@ -44079,7 +44091,7 @@
         <v>6857</v>
       </c>
       <c r="M410" s="5" t="s">
-        <v>8543</v>
+        <v>8542</v>
       </c>
     </row>
     <row r="411" spans="1:13" x14ac:dyDescent="0.4">
@@ -44120,7 +44132,7 @@
         <v>6858</v>
       </c>
       <c r="M411" s="5" t="s">
-        <v>8544</v>
+        <v>8543</v>
       </c>
     </row>
     <row r="412" spans="1:13" x14ac:dyDescent="0.4">
@@ -44161,7 +44173,7 @@
         <v>6859</v>
       </c>
       <c r="M412" s="5" t="s">
-        <v>8545</v>
+        <v>8544</v>
       </c>
     </row>
     <row r="413" spans="1:13" x14ac:dyDescent="0.4">
@@ -44202,7 +44214,7 @@
         <v>6860</v>
       </c>
       <c r="M413" s="5" t="s">
-        <v>8546</v>
+        <v>8545</v>
       </c>
     </row>
     <row r="414" spans="1:13" x14ac:dyDescent="0.4">
@@ -44243,7 +44255,7 @@
         <v>6861</v>
       </c>
       <c r="M414" s="5" t="s">
-        <v>8547</v>
+        <v>8546</v>
       </c>
     </row>
     <row r="415" spans="1:13" x14ac:dyDescent="0.4">
@@ -44284,7 +44296,7 @@
         <v>6862</v>
       </c>
       <c r="M415" s="5" t="s">
-        <v>8548</v>
+        <v>8547</v>
       </c>
     </row>
     <row r="416" spans="1:13" x14ac:dyDescent="0.4">
@@ -44325,7 +44337,7 @@
         <v>6863</v>
       </c>
       <c r="M416" s="5" t="s">
-        <v>8549</v>
+        <v>8548</v>
       </c>
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.4">
@@ -44407,7 +44419,7 @@
         <v>6864</v>
       </c>
       <c r="M418" s="5" t="s">
-        <v>8550</v>
+        <v>8549</v>
       </c>
     </row>
     <row r="419" spans="1:13" x14ac:dyDescent="0.4">
@@ -44448,7 +44460,7 @@
         <v>6865</v>
       </c>
       <c r="M419" s="5" t="s">
-        <v>8917</v>
+        <v>8916</v>
       </c>
     </row>
     <row r="420" spans="1:13" x14ac:dyDescent="0.4">
@@ -44489,7 +44501,7 @@
         <v>6866</v>
       </c>
       <c r="M420" s="5" t="s">
-        <v>8918</v>
+        <v>8917</v>
       </c>
     </row>
     <row r="421" spans="1:13" x14ac:dyDescent="0.4">
@@ -44530,7 +44542,7 @@
         <v>6867</v>
       </c>
       <c r="M421" s="5" t="s">
-        <v>8551</v>
+        <v>8550</v>
       </c>
     </row>
     <row r="422" spans="1:13" x14ac:dyDescent="0.4">
@@ -44571,7 +44583,7 @@
         <v>6868</v>
       </c>
       <c r="M422" s="5" t="s">
-        <v>8552</v>
+        <v>8551</v>
       </c>
     </row>
     <row r="423" spans="1:13" x14ac:dyDescent="0.4">
@@ -44612,7 +44624,7 @@
         <v>6869</v>
       </c>
       <c r="M423" s="5" t="s">
-        <v>8919</v>
+        <v>8918</v>
       </c>
     </row>
     <row r="424" spans="1:13" x14ac:dyDescent="0.4">
@@ -44653,7 +44665,7 @@
         <v>6870</v>
       </c>
       <c r="M424" s="5" t="s">
-        <v>8920</v>
+        <v>8919</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.4">
@@ -44694,7 +44706,7 @@
         <v>6871</v>
       </c>
       <c r="M425" s="5" t="s">
-        <v>8553</v>
+        <v>8552</v>
       </c>
     </row>
     <row r="426" spans="1:13" x14ac:dyDescent="0.4">
@@ -44735,7 +44747,7 @@
         <v>6872</v>
       </c>
       <c r="M426" s="5" t="s">
-        <v>8554</v>
+        <v>8553</v>
       </c>
     </row>
     <row r="427" spans="1:13" x14ac:dyDescent="0.4">
@@ -44776,7 +44788,7 @@
         <v>6873</v>
       </c>
       <c r="M427" s="5" t="s">
-        <v>8555</v>
+        <v>8554</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.4">
@@ -44817,7 +44829,7 @@
         <v>6874</v>
       </c>
       <c r="M428" s="5" t="s">
-        <v>8556</v>
+        <v>8555</v>
       </c>
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.4">
@@ -44858,7 +44870,7 @@
         <v>6875</v>
       </c>
       <c r="M429" s="5" t="s">
-        <v>8557</v>
+        <v>8556</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.4">
@@ -44899,7 +44911,7 @@
         <v>6876</v>
       </c>
       <c r="M430" s="5" t="s">
-        <v>8558</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.4">
@@ -44940,7 +44952,7 @@
         <v>6877</v>
       </c>
       <c r="M431" s="5" t="s">
-        <v>8559</v>
+        <v>8558</v>
       </c>
     </row>
     <row r="432" spans="1:13" x14ac:dyDescent="0.4">
@@ -44981,7 +44993,7 @@
         <v>6878</v>
       </c>
       <c r="M432" s="5" t="s">
-        <v>8560</v>
+        <v>8559</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.4">
@@ -45022,7 +45034,7 @@
         <v>6879</v>
       </c>
       <c r="M433" s="5" t="s">
-        <v>8801</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="434" spans="1:13" x14ac:dyDescent="0.4">
@@ -45063,7 +45075,7 @@
         <v>6880</v>
       </c>
       <c r="M434" s="5" t="s">
-        <v>8561</v>
+        <v>8560</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.4">
@@ -45104,7 +45116,7 @@
         <v>6881</v>
       </c>
       <c r="M435" s="5" t="s">
-        <v>8786</v>
+        <v>8785</v>
       </c>
     </row>
     <row r="436" spans="1:13" x14ac:dyDescent="0.4">
@@ -45145,7 +45157,7 @@
         <v>6882</v>
       </c>
       <c r="M436" s="5" t="s">
-        <v>8562</v>
+        <v>8561</v>
       </c>
     </row>
     <row r="437" spans="1:13" x14ac:dyDescent="0.4">
@@ -45186,7 +45198,7 @@
         <v>6883</v>
       </c>
       <c r="M437" s="5" t="s">
-        <v>8563</v>
+        <v>8562</v>
       </c>
     </row>
     <row r="438" spans="1:13" x14ac:dyDescent="0.4">
@@ -45227,7 +45239,7 @@
         <v>6884</v>
       </c>
       <c r="M438" s="5" t="s">
-        <v>8564</v>
+        <v>8563</v>
       </c>
     </row>
     <row r="439" spans="1:13" x14ac:dyDescent="0.4">
@@ -45268,7 +45280,7 @@
         <v>6885</v>
       </c>
       <c r="M439" s="5" t="s">
-        <v>8565</v>
+        <v>8564</v>
       </c>
     </row>
     <row r="440" spans="1:13" x14ac:dyDescent="0.4">
@@ -45309,7 +45321,7 @@
         <v>6886</v>
       </c>
       <c r="M440" s="5" t="s">
-        <v>8566</v>
+        <v>8565</v>
       </c>
     </row>
     <row r="441" spans="1:13" x14ac:dyDescent="0.4">
@@ -45350,7 +45362,7 @@
         <v>6887</v>
       </c>
       <c r="M441" s="5" t="s">
-        <v>8921</v>
+        <v>8920</v>
       </c>
     </row>
     <row r="442" spans="1:13" x14ac:dyDescent="0.4">
@@ -45391,7 +45403,7 @@
         <v>6888</v>
       </c>
       <c r="M442" s="5" t="s">
-        <v>8567</v>
+        <v>8566</v>
       </c>
     </row>
     <row r="443" spans="1:13" x14ac:dyDescent="0.4">
@@ -45432,7 +45444,7 @@
         <v>6889</v>
       </c>
       <c r="M443" s="5" t="s">
-        <v>8568</v>
+        <v>8567</v>
       </c>
     </row>
     <row r="444" spans="1:13" x14ac:dyDescent="0.4">
@@ -45473,7 +45485,7 @@
         <v>6890</v>
       </c>
       <c r="M444" s="5" t="s">
-        <v>8569</v>
+        <v>8568</v>
       </c>
     </row>
     <row r="445" spans="1:13" x14ac:dyDescent="0.4">
@@ -45514,7 +45526,7 @@
         <v>6891</v>
       </c>
       <c r="M445" s="5" t="s">
-        <v>8922</v>
+        <v>8921</v>
       </c>
     </row>
     <row r="446" spans="1:13" x14ac:dyDescent="0.4">
@@ -45555,7 +45567,7 @@
         <v>6892</v>
       </c>
       <c r="M446" s="5" t="s">
-        <v>8923</v>
+        <v>8922</v>
       </c>
     </row>
     <row r="447" spans="1:13" x14ac:dyDescent="0.4">
@@ -45596,7 +45608,7 @@
         <v>6893</v>
       </c>
       <c r="M447" s="5" t="s">
-        <v>8787</v>
+        <v>8786</v>
       </c>
     </row>
     <row r="448" spans="1:13" x14ac:dyDescent="0.4">
@@ -45637,7 +45649,7 @@
         <v>6894</v>
       </c>
       <c r="M448" s="5" t="s">
-        <v>8570</v>
+        <v>8569</v>
       </c>
     </row>
     <row r="449" spans="1:13" x14ac:dyDescent="0.4">
@@ -45678,7 +45690,7 @@
         <v>6895</v>
       </c>
       <c r="M449" s="5" t="s">
-        <v>8571</v>
+        <v>8570</v>
       </c>
     </row>
     <row r="450" spans="1:13" x14ac:dyDescent="0.4">
@@ -45719,7 +45731,7 @@
         <v>6896</v>
       </c>
       <c r="M450" s="5" t="s">
-        <v>8788</v>
+        <v>8787</v>
       </c>
     </row>
     <row r="451" spans="1:13" x14ac:dyDescent="0.4">
@@ -45760,7 +45772,7 @@
         <v>6897</v>
       </c>
       <c r="M451" s="5" t="s">
-        <v>8572</v>
+        <v>8571</v>
       </c>
     </row>
     <row r="452" spans="1:13" x14ac:dyDescent="0.4">
@@ -45801,7 +45813,7 @@
         <v>6898</v>
       </c>
       <c r="M452" s="5" t="s">
-        <v>8573</v>
+        <v>8572</v>
       </c>
     </row>
     <row r="453" spans="1:13" x14ac:dyDescent="0.4">
@@ -45842,7 +45854,7 @@
         <v>6899</v>
       </c>
       <c r="M453" s="5" t="s">
-        <v>8574</v>
+        <v>8573</v>
       </c>
     </row>
     <row r="454" spans="1:13" x14ac:dyDescent="0.4">
@@ -45883,7 +45895,7 @@
         <v>6900</v>
       </c>
       <c r="M454" s="5" t="s">
-        <v>8575</v>
+        <v>8574</v>
       </c>
     </row>
     <row r="455" spans="1:13" x14ac:dyDescent="0.4">
@@ -45924,7 +45936,7 @@
         <v>6814</v>
       </c>
       <c r="M455" s="5" t="s">
-        <v>8789</v>
+        <v>8788</v>
       </c>
     </row>
     <row r="456" spans="1:13" x14ac:dyDescent="0.4">
@@ -45965,7 +45977,7 @@
         <v>6901</v>
       </c>
       <c r="M456" s="5" t="s">
-        <v>8576</v>
+        <v>8575</v>
       </c>
     </row>
     <row r="457" spans="1:13" x14ac:dyDescent="0.4">
@@ -46006,7 +46018,7 @@
         <v>6902</v>
       </c>
       <c r="M457" s="5" t="s">
-        <v>8790</v>
+        <v>8789</v>
       </c>
     </row>
     <row r="458" spans="1:13" x14ac:dyDescent="0.4">
@@ -46047,7 +46059,7 @@
         <v>6903</v>
       </c>
       <c r="M458" s="5" t="s">
-        <v>8791</v>
+        <v>8790</v>
       </c>
     </row>
     <row r="459" spans="1:13" x14ac:dyDescent="0.4">
@@ -46088,7 +46100,7 @@
         <v>6904</v>
       </c>
       <c r="M459" s="5" t="s">
-        <v>8577</v>
+        <v>8576</v>
       </c>
     </row>
     <row r="460" spans="1:13" x14ac:dyDescent="0.4">
@@ -46129,7 +46141,7 @@
         <v>6905</v>
       </c>
       <c r="M460" s="5" t="s">
-        <v>8578</v>
+        <v>8577</v>
       </c>
     </row>
     <row r="461" spans="1:13" x14ac:dyDescent="0.4">
@@ -46170,7 +46182,7 @@
         <v>6906</v>
       </c>
       <c r="M461" s="5" t="s">
-        <v>8579</v>
+        <v>8578</v>
       </c>
     </row>
     <row r="462" spans="1:13" x14ac:dyDescent="0.4">
@@ -46211,7 +46223,7 @@
         <v>6907</v>
       </c>
       <c r="M462" s="5" t="s">
-        <v>8580</v>
+        <v>8579</v>
       </c>
     </row>
     <row r="463" spans="1:13" x14ac:dyDescent="0.4">
@@ -46252,7 +46264,7 @@
         <v>6908</v>
       </c>
       <c r="M463" s="5" t="s">
-        <v>8581</v>
+        <v>8580</v>
       </c>
     </row>
     <row r="464" spans="1:13" x14ac:dyDescent="0.4">
@@ -46293,7 +46305,7 @@
         <v>6909</v>
       </c>
       <c r="M464" s="5" t="s">
-        <v>8582</v>
+        <v>8581</v>
       </c>
     </row>
     <row r="465" spans="1:13" x14ac:dyDescent="0.4">
@@ -46334,7 +46346,7 @@
         <v>2436</v>
       </c>
       <c r="M465" s="5" t="s">
-        <v>8583</v>
+        <v>8582</v>
       </c>
     </row>
     <row r="466" spans="1:13" x14ac:dyDescent="0.4">
@@ -46375,7 +46387,7 @@
         <v>6910</v>
       </c>
       <c r="M466" s="5" t="s">
-        <v>8881</v>
+        <v>8880</v>
       </c>
     </row>
     <row r="467" spans="1:13" x14ac:dyDescent="0.4">
@@ -46416,7 +46428,7 @@
         <v>6911</v>
       </c>
       <c r="M467" s="5" t="s">
-        <v>8792</v>
+        <v>8791</v>
       </c>
     </row>
     <row r="468" spans="1:13" x14ac:dyDescent="0.4">
@@ -46457,7 +46469,7 @@
         <v>2439</v>
       </c>
       <c r="M468" s="5" t="s">
-        <v>8584</v>
+        <v>8583</v>
       </c>
     </row>
     <row r="469" spans="1:13" x14ac:dyDescent="0.4">
@@ -46471,7 +46483,7 @@
         <v>1794</v>
       </c>
       <c r="D469" t="s">
-        <v>8783</v>
+        <v>8782</v>
       </c>
       <c r="E469" t="s">
         <v>3082</v>
@@ -46498,7 +46510,7 @@
         <v>6912</v>
       </c>
       <c r="M469" s="5" t="s">
-        <v>8882</v>
+        <v>8881</v>
       </c>
     </row>
     <row r="470" spans="1:13" x14ac:dyDescent="0.4">
@@ -46539,7 +46551,7 @@
         <v>6913</v>
       </c>
       <c r="M470" s="5" t="s">
-        <v>8585</v>
+        <v>8584</v>
       </c>
     </row>
     <row r="471" spans="1:13" x14ac:dyDescent="0.4">
@@ -46580,7 +46592,7 @@
         <v>6914</v>
       </c>
       <c r="M471" s="5" t="s">
-        <v>8586</v>
+        <v>8585</v>
       </c>
     </row>
     <row r="472" spans="1:13" x14ac:dyDescent="0.4">
@@ -46621,7 +46633,7 @@
         <v>6915</v>
       </c>
       <c r="M472" s="5" t="s">
-        <v>8587</v>
+        <v>8586</v>
       </c>
     </row>
     <row r="473" spans="1:13" x14ac:dyDescent="0.4">
@@ -46662,7 +46674,7 @@
         <v>6916</v>
       </c>
       <c r="M473" s="5" t="s">
-        <v>8588</v>
+        <v>8587</v>
       </c>
     </row>
     <row r="474" spans="1:13" x14ac:dyDescent="0.4">
@@ -46703,7 +46715,7 @@
         <v>6917</v>
       </c>
       <c r="M474" s="5" t="s">
-        <v>8589</v>
+        <v>8588</v>
       </c>
     </row>
     <row r="475" spans="1:13" x14ac:dyDescent="0.4">
@@ -46744,7 +46756,7 @@
         <v>6918</v>
       </c>
       <c r="M475" s="5" t="s">
-        <v>8590</v>
+        <v>8589</v>
       </c>
     </row>
     <row r="476" spans="1:13" x14ac:dyDescent="0.4">
@@ -46785,7 +46797,7 @@
         <v>8232</v>
       </c>
       <c r="M476" s="5" t="s">
-        <v>8591</v>
+        <v>8590</v>
       </c>
     </row>
     <row r="477" spans="1:13" x14ac:dyDescent="0.4">
@@ -46826,7 +46838,7 @@
         <v>6919</v>
       </c>
       <c r="M477" s="5" t="s">
-        <v>8592</v>
+        <v>8591</v>
       </c>
     </row>
     <row r="478" spans="1:13" x14ac:dyDescent="0.4">
@@ -46867,7 +46879,7 @@
         <v>6920</v>
       </c>
       <c r="M478" s="5" t="s">
-        <v>8593</v>
+        <v>8592</v>
       </c>
     </row>
     <row r="479" spans="1:13" x14ac:dyDescent="0.4">
@@ -46908,7 +46920,7 @@
         <v>6921</v>
       </c>
       <c r="M479" s="5" t="s">
-        <v>8594</v>
+        <v>8593</v>
       </c>
     </row>
     <row r="480" spans="1:13" x14ac:dyDescent="0.4">
@@ -46949,7 +46961,7 @@
         <v>6922</v>
       </c>
       <c r="M480" s="5" t="s">
-        <v>8883</v>
+        <v>8882</v>
       </c>
     </row>
     <row r="481" spans="1:13" x14ac:dyDescent="0.4">
@@ -46990,7 +47002,7 @@
         <v>5698</v>
       </c>
       <c r="M481" s="5" t="s">
-        <v>8595</v>
+        <v>8594</v>
       </c>
     </row>
     <row r="482" spans="1:13" x14ac:dyDescent="0.4">
@@ -47031,7 +47043,7 @@
         <v>6923</v>
       </c>
       <c r="M482" s="5" t="s">
-        <v>8596</v>
+        <v>8595</v>
       </c>
     </row>
     <row r="483" spans="1:13" x14ac:dyDescent="0.4">
@@ -47072,7 +47084,7 @@
         <v>6924</v>
       </c>
       <c r="M483" s="5" t="s">
-        <v>8597</v>
+        <v>8596</v>
       </c>
     </row>
     <row r="484" spans="1:13" x14ac:dyDescent="0.4">
@@ -47113,7 +47125,7 @@
         <v>6925</v>
       </c>
       <c r="M484" s="5" t="s">
-        <v>8598</v>
+        <v>8597</v>
       </c>
     </row>
     <row r="485" spans="1:13" x14ac:dyDescent="0.4">
@@ -47154,7 +47166,7 @@
         <v>6926</v>
       </c>
       <c r="M485" s="5" t="s">
-        <v>8599</v>
+        <v>8598</v>
       </c>
     </row>
     <row r="486" spans="1:13" x14ac:dyDescent="0.4">
@@ -47195,7 +47207,7 @@
         <v>6927</v>
       </c>
       <c r="M486" s="5" t="s">
-        <v>8600</v>
+        <v>8599</v>
       </c>
     </row>
     <row r="487" spans="1:13" x14ac:dyDescent="0.4">
@@ -47236,7 +47248,7 @@
         <v>6928</v>
       </c>
       <c r="M487" s="5" t="s">
-        <v>8601</v>
+        <v>8600</v>
       </c>
     </row>
     <row r="488" spans="1:13" x14ac:dyDescent="0.4">
@@ -47277,7 +47289,7 @@
         <v>6929</v>
       </c>
       <c r="M488" s="5" t="s">
-        <v>8465</v>
+        <v>8464</v>
       </c>
     </row>
     <row r="489" spans="1:13" x14ac:dyDescent="0.4">
@@ -47318,7 +47330,7 @@
         <v>6930</v>
       </c>
       <c r="M489" s="5" t="s">
-        <v>8602</v>
+        <v>8601</v>
       </c>
     </row>
     <row r="490" spans="1:13" x14ac:dyDescent="0.4">
@@ -47359,7 +47371,7 @@
         <v>6931</v>
       </c>
       <c r="M490" s="5" t="s">
-        <v>8603</v>
+        <v>8602</v>
       </c>
     </row>
     <row r="491" spans="1:13" x14ac:dyDescent="0.4">
@@ -47400,7 +47412,7 @@
         <v>6932</v>
       </c>
       <c r="M491" s="5" t="s">
-        <v>8604</v>
+        <v>8603</v>
       </c>
     </row>
     <row r="492" spans="1:13" x14ac:dyDescent="0.4">
@@ -47441,7 +47453,7 @@
         <v>6933</v>
       </c>
       <c r="M492" s="5" t="s">
-        <v>8605</v>
+        <v>8604</v>
       </c>
     </row>
     <row r="493" spans="1:13" x14ac:dyDescent="0.4">
@@ -47482,7 +47494,7 @@
         <v>6934</v>
       </c>
       <c r="M493" s="5" t="s">
-        <v>8606</v>
+        <v>8605</v>
       </c>
     </row>
     <row r="494" spans="1:13" x14ac:dyDescent="0.4">
@@ -47523,7 +47535,7 @@
         <v>6935</v>
       </c>
       <c r="M494" s="5" t="s">
-        <v>8607</v>
+        <v>8606</v>
       </c>
     </row>
     <row r="495" spans="1:13" x14ac:dyDescent="0.4">
@@ -47564,7 +47576,7 @@
         <v>6936</v>
       </c>
       <c r="M495" s="5" t="s">
-        <v>8608</v>
+        <v>8607</v>
       </c>
     </row>
     <row r="496" spans="1:13" x14ac:dyDescent="0.4">
@@ -47605,7 +47617,7 @@
         <v>6937</v>
       </c>
       <c r="M496" s="5" t="s">
-        <v>8609</v>
+        <v>8608</v>
       </c>
     </row>
     <row r="497" spans="1:13" x14ac:dyDescent="0.4">
@@ -47646,7 +47658,7 @@
         <v>6938</v>
       </c>
       <c r="M497" s="5" t="s">
-        <v>8610</v>
+        <v>8609</v>
       </c>
     </row>
     <row r="498" spans="1:13" x14ac:dyDescent="0.4">
@@ -47687,7 +47699,7 @@
         <v>6939</v>
       </c>
       <c r="M498" s="5" t="s">
-        <v>8611</v>
+        <v>8610</v>
       </c>
     </row>
     <row r="499" spans="1:13" x14ac:dyDescent="0.4">
@@ -47728,7 +47740,7 @@
         <v>6940</v>
       </c>
       <c r="M499" s="5" t="s">
-        <v>8612</v>
+        <v>8611</v>
       </c>
     </row>
     <row r="500" spans="1:13" x14ac:dyDescent="0.4">
@@ -47769,7 +47781,7 @@
         <v>6941</v>
       </c>
       <c r="M500" s="5" t="s">
-        <v>8884</v>
+        <v>8883</v>
       </c>
     </row>
     <row r="501" spans="1:13" x14ac:dyDescent="0.4">
@@ -47810,7 +47822,7 @@
         <v>6942</v>
       </c>
       <c r="M501" s="5" t="s">
-        <v>8613</v>
+        <v>8612</v>
       </c>
     </row>
     <row r="502" spans="1:13" x14ac:dyDescent="0.4">
@@ -47851,7 +47863,7 @@
         <v>6943</v>
       </c>
       <c r="M502" s="5" t="s">
-        <v>8614</v>
+        <v>8613</v>
       </c>
     </row>
     <row r="503" spans="1:13" x14ac:dyDescent="0.4">
@@ -47892,7 +47904,7 @@
         <v>6944</v>
       </c>
       <c r="M503" s="5" t="s">
-        <v>8615</v>
+        <v>8614</v>
       </c>
     </row>
     <row r="504" spans="1:13" x14ac:dyDescent="0.4">
@@ -47933,7 +47945,7 @@
         <v>6945</v>
       </c>
       <c r="M504" s="5" t="s">
-        <v>8885</v>
+        <v>8884</v>
       </c>
     </row>
     <row r="505" spans="1:13" x14ac:dyDescent="0.4">
@@ -47974,7 +47986,7 @@
         <v>6946</v>
       </c>
       <c r="M505" s="5" t="s">
-        <v>8924</v>
+        <v>8923</v>
       </c>
     </row>
     <row r="506" spans="1:13" x14ac:dyDescent="0.4">
@@ -48015,7 +48027,7 @@
         <v>6947</v>
       </c>
       <c r="M506" s="5" t="s">
-        <v>8925</v>
+        <v>8924</v>
       </c>
     </row>
     <row r="507" spans="1:13" x14ac:dyDescent="0.4">
@@ -48056,7 +48068,7 @@
         <v>6948</v>
       </c>
       <c r="M507" s="5" t="s">
-        <v>8926</v>
+        <v>8925</v>
       </c>
     </row>
     <row r="508" spans="1:13" x14ac:dyDescent="0.4">
@@ -48097,7 +48109,7 @@
         <v>5725</v>
       </c>
       <c r="M508" s="5" t="s">
-        <v>8616</v>
+        <v>8615</v>
       </c>
     </row>
     <row r="509" spans="1:13" x14ac:dyDescent="0.4">
@@ -48138,7 +48150,7 @@
         <v>6949</v>
       </c>
       <c r="M509" s="5" t="s">
-        <v>8617</v>
+        <v>8616</v>
       </c>
     </row>
     <row r="510" spans="1:13" x14ac:dyDescent="0.4">
@@ -48179,7 +48191,7 @@
         <v>6950</v>
       </c>
       <c r="M510" s="5" t="s">
-        <v>8618</v>
+        <v>8617</v>
       </c>
     </row>
     <row r="511" spans="1:13" x14ac:dyDescent="0.4">
@@ -48220,7 +48232,7 @@
         <v>6951</v>
       </c>
       <c r="M511" s="5" t="s">
-        <v>8619</v>
+        <v>8618</v>
       </c>
     </row>
     <row r="512" spans="1:13" x14ac:dyDescent="0.4">
@@ -48261,7 +48273,7 @@
         <v>6952</v>
       </c>
       <c r="M512" s="5" t="s">
-        <v>8620</v>
+        <v>8619</v>
       </c>
     </row>
     <row r="513" spans="1:13" x14ac:dyDescent="0.4">
@@ -48302,7 +48314,7 @@
         <v>6953</v>
       </c>
       <c r="M513" s="5" t="s">
-        <v>8621</v>
+        <v>8620</v>
       </c>
     </row>
     <row r="514" spans="1:13" x14ac:dyDescent="0.4">
@@ -48343,7 +48355,7 @@
         <v>6954</v>
       </c>
       <c r="M514" s="5" t="s">
-        <v>8622</v>
+        <v>8621</v>
       </c>
     </row>
     <row r="515" spans="1:13" x14ac:dyDescent="0.4">
@@ -48425,7 +48437,7 @@
         <v>6956</v>
       </c>
       <c r="M516" s="5" t="s">
-        <v>8623</v>
+        <v>8622</v>
       </c>
     </row>
     <row r="517" spans="1:13" x14ac:dyDescent="0.4">
@@ -48466,7 +48478,7 @@
         <v>6957</v>
       </c>
       <c r="M517" s="5" t="s">
-        <v>8624</v>
+        <v>8623</v>
       </c>
     </row>
     <row r="518" spans="1:13" x14ac:dyDescent="0.4">
@@ -48507,7 +48519,7 @@
         <v>6958</v>
       </c>
       <c r="M518" s="5" t="s">
-        <v>8625</v>
+        <v>8624</v>
       </c>
     </row>
     <row r="519" spans="1:13" x14ac:dyDescent="0.4">
@@ -48548,7 +48560,7 @@
         <v>6959</v>
       </c>
       <c r="M519" s="5" t="s">
-        <v>8927</v>
+        <v>8926</v>
       </c>
     </row>
     <row r="520" spans="1:13" x14ac:dyDescent="0.4">
@@ -48589,7 +48601,7 @@
         <v>6960</v>
       </c>
       <c r="M520" s="5" t="s">
-        <v>8626</v>
+        <v>8625</v>
       </c>
     </row>
     <row r="521" spans="1:13" x14ac:dyDescent="0.4">
@@ -48630,7 +48642,7 @@
         <v>6961</v>
       </c>
       <c r="M521" s="5" t="s">
-        <v>8886</v>
+        <v>8885</v>
       </c>
     </row>
     <row r="522" spans="1:13" x14ac:dyDescent="0.4">
@@ -48671,7 +48683,7 @@
         <v>6962</v>
       </c>
       <c r="M522" s="5" t="s">
-        <v>8627</v>
+        <v>8626</v>
       </c>
     </row>
     <row r="523" spans="1:13" x14ac:dyDescent="0.4">
@@ -48712,7 +48724,7 @@
         <v>6963</v>
       </c>
       <c r="M523" s="5" t="s">
-        <v>8928</v>
+        <v>8927</v>
       </c>
     </row>
     <row r="524" spans="1:13" x14ac:dyDescent="0.4">
@@ -48753,7 +48765,7 @@
         <v>6964</v>
       </c>
       <c r="M524" s="5" t="s">
-        <v>8929</v>
+        <v>8928</v>
       </c>
     </row>
     <row r="525" spans="1:13" x14ac:dyDescent="0.4">
@@ -48794,7 +48806,7 @@
         <v>6965</v>
       </c>
       <c r="M525" s="5" t="s">
-        <v>8628</v>
+        <v>8627</v>
       </c>
     </row>
     <row r="526" spans="1:13" x14ac:dyDescent="0.4">
@@ -48835,7 +48847,7 @@
         <v>6966</v>
       </c>
       <c r="M526" s="5" t="s">
-        <v>8629</v>
+        <v>8628</v>
       </c>
     </row>
     <row r="527" spans="1:13" x14ac:dyDescent="0.4">
@@ -48876,7 +48888,7 @@
         <v>6967</v>
       </c>
       <c r="M527" s="5" t="s">
-        <v>8630</v>
+        <v>8629</v>
       </c>
     </row>
     <row r="528" spans="1:13" x14ac:dyDescent="0.4">
@@ -48917,7 +48929,7 @@
         <v>5745</v>
       </c>
       <c r="M528" s="5" t="s">
-        <v>8887</v>
+        <v>8886</v>
       </c>
     </row>
     <row r="529" spans="1:13" x14ac:dyDescent="0.4">
@@ -48958,7 +48970,7 @@
         <v>6968</v>
       </c>
       <c r="M529" s="5" t="s">
-        <v>8631</v>
+        <v>8630</v>
       </c>
     </row>
     <row r="530" spans="1:13" x14ac:dyDescent="0.4">
@@ -48999,7 +49011,7 @@
         <v>6969</v>
       </c>
       <c r="M530" s="5" t="s">
-        <v>8632</v>
+        <v>8631</v>
       </c>
     </row>
     <row r="531" spans="1:13" x14ac:dyDescent="0.4">
@@ -49040,7 +49052,7 @@
         <v>6970</v>
       </c>
       <c r="M531" s="5" t="s">
-        <v>8633</v>
+        <v>8632</v>
       </c>
     </row>
     <row r="532" spans="1:13" x14ac:dyDescent="0.4">
@@ -49081,7 +49093,7 @@
         <v>6971</v>
       </c>
       <c r="M532" s="5" t="s">
-        <v>8634</v>
+        <v>8633</v>
       </c>
     </row>
     <row r="533" spans="1:13" x14ac:dyDescent="0.4">
@@ -49122,7 +49134,7 @@
         <v>6972</v>
       </c>
       <c r="M533" s="5" t="s">
-        <v>8635</v>
+        <v>8634</v>
       </c>
     </row>
     <row r="534" spans="1:13" x14ac:dyDescent="0.4">
@@ -49163,7 +49175,7 @@
         <v>6973</v>
       </c>
       <c r="M534" s="5" t="s">
-        <v>8888</v>
+        <v>8887</v>
       </c>
     </row>
     <row r="535" spans="1:13" x14ac:dyDescent="0.4">
@@ -49204,7 +49216,7 @@
         <v>6974</v>
       </c>
       <c r="M535" s="5" t="s">
-        <v>8636</v>
+        <v>8635</v>
       </c>
     </row>
     <row r="536" spans="1:13" x14ac:dyDescent="0.4">
@@ -49245,7 +49257,7 @@
         <v>6781</v>
       </c>
       <c r="M536" s="5" t="s">
-        <v>8889</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="537" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49286,7 +49298,7 @@
         <v>6975</v>
       </c>
       <c r="M537" s="5" t="s">
-        <v>8637</v>
+        <v>8636</v>
       </c>
     </row>
     <row r="538" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49327,7 +49339,7 @@
         <v>6976</v>
       </c>
       <c r="M538" s="5" t="s">
-        <v>8638</v>
+        <v>8637</v>
       </c>
     </row>
     <row r="539" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49368,7 +49380,7 @@
         <v>6977</v>
       </c>
       <c r="M539" s="5" t="s">
-        <v>8639</v>
+        <v>8638</v>
       </c>
     </row>
     <row r="540" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49409,7 +49421,7 @@
         <v>6978</v>
       </c>
       <c r="M540" s="5" t="s">
-        <v>8640</v>
+        <v>8639</v>
       </c>
     </row>
     <row r="541" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49450,7 +49462,7 @@
         <v>6979</v>
       </c>
       <c r="M541" s="5" t="s">
-        <v>8641</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="542" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49491,7 +49503,7 @@
         <v>8003</v>
       </c>
       <c r="M542" s="5" t="s">
-        <v>8890</v>
+        <v>8889</v>
       </c>
     </row>
     <row r="543" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49532,7 +49544,7 @@
         <v>8004</v>
       </c>
       <c r="M543" s="5" t="s">
-        <v>8642</v>
+        <v>8641</v>
       </c>
     </row>
     <row r="544" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49573,7 +49585,7 @@
         <v>8005</v>
       </c>
       <c r="M544" s="5" t="s">
-        <v>8643</v>
+        <v>8642</v>
       </c>
     </row>
     <row r="545" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -49614,7 +49626,7 @@
         <v>8006</v>
       </c>
       <c r="M545" s="5" t="s">
-        <v>8644</v>
+        <v>8643</v>
       </c>
     </row>
     <row r="546" spans="1:13" x14ac:dyDescent="0.4">
@@ -49655,7 +49667,7 @@
         <v>5758</v>
       </c>
       <c r="M546" s="5" t="s">
-        <v>8891</v>
+        <v>8890</v>
       </c>
     </row>
     <row r="547" spans="1:13" x14ac:dyDescent="0.4">
@@ -49696,7 +49708,7 @@
         <v>6980</v>
       </c>
       <c r="M547" s="5" t="s">
-        <v>8802</v>
+        <v>8801</v>
       </c>
     </row>
     <row r="548" spans="1:13" x14ac:dyDescent="0.4">
@@ -49737,7 +49749,7 @@
         <v>6981</v>
       </c>
       <c r="M548" s="5" t="s">
-        <v>8645</v>
+        <v>8644</v>
       </c>
     </row>
     <row r="549" spans="1:13" x14ac:dyDescent="0.4">
@@ -49778,7 +49790,7 @@
         <v>6982</v>
       </c>
       <c r="M549" s="5" t="s">
-        <v>8892</v>
+        <v>8891</v>
       </c>
     </row>
     <row r="550" spans="1:13" x14ac:dyDescent="0.4">
@@ -49819,7 +49831,7 @@
         <v>6983</v>
       </c>
       <c r="M550" s="5" t="s">
-        <v>8893</v>
+        <v>8892</v>
       </c>
     </row>
     <row r="551" spans="1:13" x14ac:dyDescent="0.4">
@@ -49860,7 +49872,7 @@
         <v>6984</v>
       </c>
       <c r="M551" s="5" t="s">
-        <v>8894</v>
+        <v>8893</v>
       </c>
     </row>
     <row r="552" spans="1:13" x14ac:dyDescent="0.4">
@@ -49901,7 +49913,7 @@
         <v>6985</v>
       </c>
       <c r="M552" s="5" t="s">
-        <v>8646</v>
+        <v>8645</v>
       </c>
     </row>
     <row r="553" spans="1:13" x14ac:dyDescent="0.4">
@@ -49942,7 +49954,7 @@
         <v>6986</v>
       </c>
       <c r="M553" s="5" t="s">
-        <v>8647</v>
+        <v>8646</v>
       </c>
     </row>
     <row r="554" spans="1:13" x14ac:dyDescent="0.4">
@@ -49983,7 +49995,7 @@
         <v>6987</v>
       </c>
       <c r="M554" s="5" t="s">
-        <v>8648</v>
+        <v>8647</v>
       </c>
     </row>
     <row r="555" spans="1:13" x14ac:dyDescent="0.4">
@@ -50024,7 +50036,7 @@
         <v>6988</v>
       </c>
       <c r="M555" s="5" t="s">
-        <v>8649</v>
+        <v>8648</v>
       </c>
     </row>
     <row r="556" spans="1:13" x14ac:dyDescent="0.4">
@@ -50065,7 +50077,7 @@
         <v>6989</v>
       </c>
       <c r="M556" s="5" t="s">
-        <v>8650</v>
+        <v>8649</v>
       </c>
     </row>
     <row r="557" spans="1:13" x14ac:dyDescent="0.4">
@@ -50106,7 +50118,7 @@
         <v>7913</v>
       </c>
       <c r="M557" s="5" t="s">
-        <v>8651</v>
+        <v>8650</v>
       </c>
     </row>
     <row r="558" spans="1:13" x14ac:dyDescent="0.4">
@@ -50147,7 +50159,7 @@
         <v>7914</v>
       </c>
       <c r="M558" s="5" t="s">
-        <v>8652</v>
+        <v>8651</v>
       </c>
     </row>
     <row r="559" spans="1:13" x14ac:dyDescent="0.4">
@@ -50188,7 +50200,7 @@
         <v>7915</v>
       </c>
       <c r="M559" s="5" t="s">
-        <v>8653</v>
+        <v>8652</v>
       </c>
     </row>
     <row r="560" spans="1:13" x14ac:dyDescent="0.4">
@@ -50229,7 +50241,7 @@
         <v>7916</v>
       </c>
       <c r="M560" s="5" t="s">
-        <v>8654</v>
+        <v>8653</v>
       </c>
     </row>
     <row r="561" spans="1:13" x14ac:dyDescent="0.4">
@@ -50270,7 +50282,7 @@
         <v>6990</v>
       </c>
       <c r="M561" s="5" t="s">
-        <v>8930</v>
+        <v>8929</v>
       </c>
     </row>
     <row r="562" spans="1:13" x14ac:dyDescent="0.4">
@@ -50311,7 +50323,7 @@
         <v>6991</v>
       </c>
       <c r="M562" s="5" t="s">
-        <v>8655</v>
+        <v>8654</v>
       </c>
     </row>
     <row r="563" spans="1:13" x14ac:dyDescent="0.4">
@@ -50352,7 +50364,7 @@
         <v>7857</v>
       </c>
       <c r="M563" s="5" t="s">
-        <v>8656</v>
+        <v>8655</v>
       </c>
     </row>
     <row r="564" spans="1:13" x14ac:dyDescent="0.4">
@@ -50393,7 +50405,7 @@
         <v>7858</v>
       </c>
       <c r="M564" s="5" t="s">
-        <v>8657</v>
+        <v>8656</v>
       </c>
     </row>
     <row r="565" spans="1:13" x14ac:dyDescent="0.4">
@@ -50434,7 +50446,7 @@
         <v>6992</v>
       </c>
       <c r="M565" s="5" t="s">
-        <v>8658</v>
+        <v>8657</v>
       </c>
     </row>
     <row r="566" spans="1:13" x14ac:dyDescent="0.4">
@@ -50475,7 +50487,7 @@
         <v>6993</v>
       </c>
       <c r="M566" s="5" t="s">
-        <v>8659</v>
+        <v>8658</v>
       </c>
     </row>
     <row r="567" spans="1:13" x14ac:dyDescent="0.4">
@@ -50516,7 +50528,7 @@
         <v>2519</v>
       </c>
       <c r="M567" s="5" t="s">
-        <v>8895</v>
+        <v>8894</v>
       </c>
     </row>
     <row r="568" spans="1:13" x14ac:dyDescent="0.4">
@@ -50557,7 +50569,7 @@
         <v>6994</v>
       </c>
       <c r="M568" s="5" t="s">
-        <v>8660</v>
+        <v>8659</v>
       </c>
     </row>
     <row r="569" spans="1:13" x14ac:dyDescent="0.4">
@@ -50598,7 +50610,7 @@
         <v>6995</v>
       </c>
       <c r="M569" s="5" t="s">
-        <v>8661</v>
+        <v>8660</v>
       </c>
     </row>
     <row r="570" spans="1:13" x14ac:dyDescent="0.4">
@@ -50639,7 +50651,7 @@
         <v>6996</v>
       </c>
       <c r="M570" s="5" t="s">
-        <v>8662</v>
+        <v>8661</v>
       </c>
     </row>
     <row r="571" spans="1:13" x14ac:dyDescent="0.4">
@@ -50680,7 +50692,7 @@
         <v>6997</v>
       </c>
       <c r="M571" s="5" t="s">
-        <v>8663</v>
+        <v>8662</v>
       </c>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.4">
@@ -50721,7 +50733,7 @@
         <v>6998</v>
       </c>
       <c r="M572" s="5" t="s">
-        <v>8664</v>
+        <v>8663</v>
       </c>
     </row>
     <row r="573" spans="1:13" x14ac:dyDescent="0.4">
@@ -50762,7 +50774,7 @@
         <v>6999</v>
       </c>
       <c r="M573" s="5" t="s">
-        <v>8665</v>
+        <v>8664</v>
       </c>
     </row>
     <row r="574" spans="1:13" x14ac:dyDescent="0.4">
@@ -50803,7 +50815,7 @@
         <v>7000</v>
       </c>
       <c r="M574" s="5" t="s">
-        <v>8666</v>
+        <v>8665</v>
       </c>
     </row>
     <row r="575" spans="1:13" x14ac:dyDescent="0.4">
@@ -50844,7 +50856,7 @@
         <v>7001</v>
       </c>
       <c r="M575" s="5" t="s">
-        <v>8667</v>
+        <v>8666</v>
       </c>
     </row>
     <row r="576" spans="1:13" x14ac:dyDescent="0.4">
@@ -50885,7 +50897,7 @@
         <v>5780</v>
       </c>
       <c r="M576" s="5" t="s">
-        <v>8668</v>
+        <v>8667</v>
       </c>
     </row>
     <row r="577" spans="1:13" x14ac:dyDescent="0.4">
@@ -50926,7 +50938,7 @@
         <v>7002</v>
       </c>
       <c r="M577" s="5" t="s">
-        <v>8803</v>
+        <v>8802</v>
       </c>
     </row>
     <row r="578" spans="1:13" x14ac:dyDescent="0.4">
@@ -50967,7 +50979,7 @@
         <v>7003</v>
       </c>
       <c r="M578" s="5" t="s">
-        <v>8804</v>
+        <v>8803</v>
       </c>
     </row>
     <row r="579" spans="1:13" x14ac:dyDescent="0.4">
@@ -51008,7 +51020,7 @@
         <v>7004</v>
       </c>
       <c r="M579" s="5" t="s">
-        <v>8805</v>
+        <v>8804</v>
       </c>
     </row>
     <row r="580" spans="1:13" x14ac:dyDescent="0.4">
@@ -51049,7 +51061,7 @@
         <v>7005</v>
       </c>
       <c r="M580" s="5" t="s">
-        <v>8669</v>
+        <v>8668</v>
       </c>
     </row>
     <row r="581" spans="1:13" x14ac:dyDescent="0.4">
@@ -51090,7 +51102,7 @@
         <v>7006</v>
       </c>
       <c r="M581" s="5" t="s">
-        <v>8670</v>
+        <v>8669</v>
       </c>
     </row>
     <row r="582" spans="1:13" x14ac:dyDescent="0.4">
@@ -51131,7 +51143,7 @@
         <v>7007</v>
       </c>
       <c r="M582" s="5" t="s">
-        <v>8671</v>
+        <v>8670</v>
       </c>
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.4">
@@ -51172,7 +51184,7 @@
         <v>7008</v>
       </c>
       <c r="M583" s="5" t="s">
-        <v>8672</v>
+        <v>8671</v>
       </c>
     </row>
     <row r="584" spans="1:13" x14ac:dyDescent="0.4">
@@ -51213,7 +51225,7 @@
         <v>7924</v>
       </c>
       <c r="M584" s="5" t="s">
-        <v>8931</v>
+        <v>8930</v>
       </c>
     </row>
     <row r="585" spans="1:13" x14ac:dyDescent="0.4">
@@ -51254,7 +51266,7 @@
         <v>2536</v>
       </c>
       <c r="M585" s="5" t="s">
-        <v>8673</v>
+        <v>8672</v>
       </c>
     </row>
     <row r="586" spans="1:13" x14ac:dyDescent="0.4">
@@ -51295,7 +51307,7 @@
         <v>7009</v>
       </c>
       <c r="M586" s="5" t="s">
-        <v>8674</v>
+        <v>8673</v>
       </c>
     </row>
     <row r="587" spans="1:13" x14ac:dyDescent="0.4">
@@ -51336,7 +51348,7 @@
         <v>7010</v>
       </c>
       <c r="M587" s="5" t="s">
-        <v>8675</v>
+        <v>8674</v>
       </c>
     </row>
     <row r="588" spans="1:13" x14ac:dyDescent="0.4">
@@ -51377,7 +51389,7 @@
         <v>7011</v>
       </c>
       <c r="M588" s="5" t="s">
-        <v>8896</v>
+        <v>8895</v>
       </c>
     </row>
     <row r="589" spans="1:13" x14ac:dyDescent="0.4">
@@ -51418,7 +51430,7 @@
         <v>7012</v>
       </c>
       <c r="M589" s="5" t="s">
-        <v>8676</v>
+        <v>8675</v>
       </c>
     </row>
     <row r="590" spans="1:13" x14ac:dyDescent="0.4">
@@ -51459,7 +51471,7 @@
         <v>7013</v>
       </c>
       <c r="M590" s="5" t="s">
-        <v>8677</v>
+        <v>8676</v>
       </c>
     </row>
     <row r="591" spans="1:13" x14ac:dyDescent="0.4">
@@ -51500,7 +51512,7 @@
         <v>7014</v>
       </c>
       <c r="M591" s="5" t="s">
-        <v>8897</v>
+        <v>8896</v>
       </c>
     </row>
     <row r="592" spans="1:13" x14ac:dyDescent="0.4">
@@ -51541,7 +51553,7 @@
         <v>7015</v>
       </c>
       <c r="M592" s="5" t="s">
-        <v>8678</v>
+        <v>8677</v>
       </c>
     </row>
     <row r="593" spans="1:13" x14ac:dyDescent="0.4">
@@ -51582,7 +51594,7 @@
         <v>7016</v>
       </c>
       <c r="M593" s="5" t="s">
-        <v>8679</v>
+        <v>8678</v>
       </c>
     </row>
     <row r="594" spans="1:13" x14ac:dyDescent="0.4">
@@ -51623,7 +51635,7 @@
         <v>7017</v>
       </c>
       <c r="M594" s="5" t="s">
-        <v>8898</v>
+        <v>8897</v>
       </c>
     </row>
     <row r="595" spans="1:13" x14ac:dyDescent="0.4">
@@ -51664,7 +51676,7 @@
         <v>7018</v>
       </c>
       <c r="M595" s="5" t="s">
-        <v>8899</v>
+        <v>8898</v>
       </c>
     </row>
     <row r="596" spans="1:13" x14ac:dyDescent="0.4">
@@ -51705,7 +51717,7 @@
         <v>7019</v>
       </c>
       <c r="M596" s="5" t="s">
-        <v>8680</v>
+        <v>8679</v>
       </c>
     </row>
     <row r="597" spans="1:13" x14ac:dyDescent="0.4">
@@ -51746,7 +51758,7 @@
         <v>7020</v>
       </c>
       <c r="M597" s="5" t="s">
-        <v>8681</v>
+        <v>8680</v>
       </c>
     </row>
     <row r="598" spans="1:13" x14ac:dyDescent="0.4">
@@ -51787,7 +51799,7 @@
         <v>7021</v>
       </c>
       <c r="M598" s="5" t="s">
-        <v>8682</v>
+        <v>8681</v>
       </c>
     </row>
     <row r="599" spans="1:13" x14ac:dyDescent="0.4">
@@ -51828,7 +51840,7 @@
         <v>7022</v>
       </c>
       <c r="M599" s="5" t="s">
-        <v>8683</v>
+        <v>8682</v>
       </c>
     </row>
     <row r="600" spans="1:13" x14ac:dyDescent="0.4">
@@ -51869,7 +51881,7 @@
         <v>5803</v>
       </c>
       <c r="M600" s="5" t="s">
-        <v>8684</v>
+        <v>8683</v>
       </c>
     </row>
     <row r="601" spans="1:13" x14ac:dyDescent="0.4">
@@ -51910,7 +51922,7 @@
         <v>7023</v>
       </c>
       <c r="M601" s="5" t="s">
-        <v>8685</v>
+        <v>8684</v>
       </c>
     </row>
     <row r="602" spans="1:13" x14ac:dyDescent="0.4">
@@ -51951,7 +51963,7 @@
         <v>7024</v>
       </c>
       <c r="M602" s="5" t="s">
-        <v>8686</v>
+        <v>8685</v>
       </c>
     </row>
     <row r="603" spans="1:13" x14ac:dyDescent="0.4">
@@ -51992,7 +52004,7 @@
         <v>7025</v>
       </c>
       <c r="M603" s="5" t="s">
-        <v>8687</v>
+        <v>8686</v>
       </c>
     </row>
     <row r="604" spans="1:13" x14ac:dyDescent="0.4">
@@ -52033,7 +52045,7 @@
         <v>7026</v>
       </c>
       <c r="M604" s="5" t="s">
-        <v>8688</v>
+        <v>8687</v>
       </c>
     </row>
     <row r="605" spans="1:13" x14ac:dyDescent="0.4">
@@ -52074,7 +52086,7 @@
         <v>7027</v>
       </c>
       <c r="M605" s="5" t="s">
-        <v>8689</v>
+        <v>8688</v>
       </c>
     </row>
     <row r="606" spans="1:13" x14ac:dyDescent="0.4">
@@ -52115,7 +52127,7 @@
         <v>7028</v>
       </c>
       <c r="M606" s="5" t="s">
-        <v>8690</v>
+        <v>8689</v>
       </c>
     </row>
     <row r="607" spans="1:13" x14ac:dyDescent="0.4">
@@ -52156,7 +52168,7 @@
         <v>7029</v>
       </c>
       <c r="M607" s="5" t="s">
-        <v>8691</v>
+        <v>8690</v>
       </c>
     </row>
     <row r="608" spans="1:13" x14ac:dyDescent="0.4">
@@ -52197,7 +52209,7 @@
         <v>7030</v>
       </c>
       <c r="M608" s="5" t="s">
-        <v>8692</v>
+        <v>8691</v>
       </c>
     </row>
     <row r="609" spans="1:13" x14ac:dyDescent="0.4">
@@ -52238,7 +52250,7 @@
         <v>7031</v>
       </c>
       <c r="M609" s="5" t="s">
-        <v>8693</v>
+        <v>8692</v>
       </c>
     </row>
     <row r="610" spans="1:13" x14ac:dyDescent="0.4">
@@ -52279,7 +52291,7 @@
         <v>7032</v>
       </c>
       <c r="M610" s="5" t="s">
-        <v>8694</v>
+        <v>8693</v>
       </c>
     </row>
     <row r="611" spans="1:13" x14ac:dyDescent="0.4">
@@ -52320,7 +52332,7 @@
         <v>7033</v>
       </c>
       <c r="M611" s="5" t="s">
-        <v>8695</v>
+        <v>8694</v>
       </c>
     </row>
     <row r="612" spans="1:13" x14ac:dyDescent="0.4">
@@ -52361,7 +52373,7 @@
         <v>7034</v>
       </c>
       <c r="M612" s="5" t="s">
-        <v>8696</v>
+        <v>8695</v>
       </c>
     </row>
     <row r="613" spans="1:13" x14ac:dyDescent="0.4">
@@ -52402,7 +52414,7 @@
         <v>7035</v>
       </c>
       <c r="M613" s="5" t="s">
-        <v>8697</v>
+        <v>8696</v>
       </c>
     </row>
     <row r="614" spans="1:13" x14ac:dyDescent="0.4">
@@ -52443,7 +52455,7 @@
         <v>7036</v>
       </c>
       <c r="M614" s="5" t="s">
-        <v>8698</v>
+        <v>8697</v>
       </c>
     </row>
     <row r="615" spans="1:13" x14ac:dyDescent="0.4">
@@ -52484,7 +52496,7 @@
         <v>7037</v>
       </c>
       <c r="M615" s="5" t="s">
-        <v>8699</v>
+        <v>8698</v>
       </c>
     </row>
     <row r="616" spans="1:13" x14ac:dyDescent="0.4">
@@ -52525,7 +52537,7 @@
         <v>7038</v>
       </c>
       <c r="M616" s="5" t="s">
-        <v>8700</v>
+        <v>8699</v>
       </c>
     </row>
     <row r="617" spans="1:13" x14ac:dyDescent="0.4">
@@ -52566,7 +52578,7 @@
         <v>7039</v>
       </c>
       <c r="M617" s="5" t="s">
-        <v>8701</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="618" spans="1:13" x14ac:dyDescent="0.4">
@@ -52607,7 +52619,7 @@
         <v>7040</v>
       </c>
       <c r="M618" s="5" t="s">
-        <v>8702</v>
+        <v>8701</v>
       </c>
     </row>
     <row r="619" spans="1:13" x14ac:dyDescent="0.4">
@@ -52648,7 +52660,7 @@
         <v>7041</v>
       </c>
       <c r="M619" s="5" t="s">
-        <v>8703</v>
+        <v>8702</v>
       </c>
     </row>
     <row r="620" spans="1:13" x14ac:dyDescent="0.4">
@@ -52689,7 +52701,7 @@
         <v>7042</v>
       </c>
       <c r="M620" s="5" t="s">
-        <v>8900</v>
+        <v>8899</v>
       </c>
     </row>
     <row r="621" spans="1:13" x14ac:dyDescent="0.4">
@@ -52730,7 +52742,7 @@
         <v>7043</v>
       </c>
       <c r="M621" s="5" t="s">
-        <v>8704</v>
+        <v>8703</v>
       </c>
     </row>
     <row r="622" spans="1:13" x14ac:dyDescent="0.4">
@@ -52771,7 +52783,7 @@
         <v>7044</v>
       </c>
       <c r="M622" s="5" t="s">
-        <v>8705</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="623" spans="1:13" x14ac:dyDescent="0.4">
@@ -52812,7 +52824,7 @@
         <v>7045</v>
       </c>
       <c r="M623" s="5" t="s">
-        <v>8706</v>
+        <v>8705</v>
       </c>
     </row>
     <row r="624" spans="1:13" x14ac:dyDescent="0.4">
@@ -52853,7 +52865,7 @@
         <v>7046</v>
       </c>
       <c r="M624" s="5" t="s">
-        <v>8707</v>
+        <v>8706</v>
       </c>
     </row>
     <row r="625" spans="1:13" x14ac:dyDescent="0.4">
@@ -52894,7 +52906,7 @@
         <v>7047</v>
       </c>
       <c r="M625" s="5" t="s">
-        <v>8708</v>
+        <v>8707</v>
       </c>
     </row>
     <row r="626" spans="1:13" x14ac:dyDescent="0.4">
@@ -52935,7 +52947,7 @@
         <v>7048</v>
       </c>
       <c r="M626" s="5" t="s">
-        <v>8709</v>
+        <v>8708</v>
       </c>
     </row>
     <row r="627" spans="1:13" x14ac:dyDescent="0.4">
@@ -52976,7 +52988,7 @@
         <v>7049</v>
       </c>
       <c r="M627" s="5" t="s">
-        <v>8901</v>
+        <v>8900</v>
       </c>
     </row>
     <row r="628" spans="1:13" x14ac:dyDescent="0.4">
@@ -53017,7 +53029,7 @@
         <v>7050</v>
       </c>
       <c r="M628" s="5" t="s">
-        <v>8710</v>
+        <v>8709</v>
       </c>
     </row>
     <row r="629" spans="1:13" x14ac:dyDescent="0.4">
@@ -53058,7 +53070,7 @@
         <v>7051</v>
       </c>
       <c r="M629" s="5" t="s">
-        <v>8711</v>
+        <v>8710</v>
       </c>
     </row>
     <row r="630" spans="1:13" x14ac:dyDescent="0.4">
@@ -53099,7 +53111,7 @@
         <v>7052</v>
       </c>
       <c r="M630" s="5" t="s">
-        <v>8712</v>
+        <v>8711</v>
       </c>
     </row>
     <row r="631" spans="1:13" x14ac:dyDescent="0.4">
@@ -53140,7 +53152,7 @@
         <v>7053</v>
       </c>
       <c r="M631" s="5" t="s">
-        <v>8713</v>
+        <v>8712</v>
       </c>
     </row>
     <row r="632" spans="1:13" x14ac:dyDescent="0.4">
@@ -53181,7 +53193,7 @@
         <v>7054</v>
       </c>
       <c r="M632" s="5" t="s">
-        <v>8714</v>
+        <v>8713</v>
       </c>
     </row>
     <row r="633" spans="1:13" x14ac:dyDescent="0.4">
@@ -53222,7 +53234,7 @@
         <v>7055</v>
       </c>
       <c r="M633" s="5" t="s">
-        <v>8715</v>
+        <v>8714</v>
       </c>
     </row>
     <row r="634" spans="1:13" x14ac:dyDescent="0.4">
@@ -53263,7 +53275,7 @@
         <v>6723</v>
       </c>
       <c r="M634" s="5" t="s">
-        <v>8716</v>
+        <v>8715</v>
       </c>
     </row>
     <row r="635" spans="1:13" x14ac:dyDescent="0.4">
@@ -53304,7 +53316,7 @@
         <v>7056</v>
       </c>
       <c r="M635" s="5" t="s">
-        <v>8717</v>
+        <v>8716</v>
       </c>
     </row>
     <row r="636" spans="1:13" x14ac:dyDescent="0.4">
@@ -53345,7 +53357,7 @@
         <v>7057</v>
       </c>
       <c r="M636" s="5" t="s">
-        <v>8718</v>
+        <v>8717</v>
       </c>
     </row>
     <row r="637" spans="1:13" x14ac:dyDescent="0.4">
@@ -53386,7 +53398,7 @@
         <v>7058</v>
       </c>
       <c r="M637" s="5" t="s">
-        <v>8719</v>
+        <v>8718</v>
       </c>
     </row>
     <row r="638" spans="1:13" x14ac:dyDescent="0.4">
@@ -53427,7 +53439,7 @@
         <v>7059</v>
       </c>
       <c r="M638" s="5" t="s">
-        <v>8720</v>
+        <v>8719</v>
       </c>
     </row>
     <row r="639" spans="1:13" x14ac:dyDescent="0.4">
@@ -53468,7 +53480,7 @@
         <v>7060</v>
       </c>
       <c r="M639" s="5" t="s">
-        <v>8721</v>
+        <v>8720</v>
       </c>
     </row>
     <row r="640" spans="1:13" x14ac:dyDescent="0.4">
@@ -53509,7 +53521,7 @@
         <v>7061</v>
       </c>
       <c r="M640" s="5" t="s">
-        <v>8722</v>
+        <v>8721</v>
       </c>
     </row>
     <row r="641" spans="1:13" x14ac:dyDescent="0.4">
@@ -53550,7 +53562,7 @@
         <v>7062</v>
       </c>
       <c r="M641" s="5" t="s">
-        <v>8723</v>
+        <v>8722</v>
       </c>
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.4">
@@ -53591,7 +53603,7 @@
         <v>7063</v>
       </c>
       <c r="M642" s="5" t="s">
-        <v>8724</v>
+        <v>8723</v>
       </c>
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.4">
@@ -53632,7 +53644,7 @@
         <v>7064</v>
       </c>
       <c r="M643" s="5" t="s">
-        <v>8725</v>
+        <v>8724</v>
       </c>
     </row>
     <row r="644" spans="1:13" x14ac:dyDescent="0.4">
@@ -53673,7 +53685,7 @@
         <v>7065</v>
       </c>
       <c r="M644" s="5" t="s">
-        <v>8726</v>
+        <v>8725</v>
       </c>
     </row>
     <row r="645" spans="1:13" x14ac:dyDescent="0.4">
@@ -53714,7 +53726,7 @@
         <v>7066</v>
       </c>
       <c r="M645" s="5" t="s">
-        <v>8727</v>
+        <v>8726</v>
       </c>
     </row>
     <row r="646" spans="1:13" x14ac:dyDescent="0.4">
@@ -53755,7 +53767,7 @@
         <v>7067</v>
       </c>
       <c r="M646" s="5" t="s">
-        <v>8728</v>
+        <v>8727</v>
       </c>
     </row>
     <row r="647" spans="1:13" x14ac:dyDescent="0.4">
@@ -53796,7 +53808,7 @@
         <v>7068</v>
       </c>
       <c r="M647" s="5" t="s">
-        <v>8729</v>
+        <v>8728</v>
       </c>
     </row>
     <row r="648" spans="1:13" x14ac:dyDescent="0.4">
@@ -53837,7 +53849,7 @@
         <v>7069</v>
       </c>
       <c r="M648" s="5" t="s">
-        <v>8730</v>
+        <v>8729</v>
       </c>
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.4">
@@ -53878,7 +53890,7 @@
         <v>7070</v>
       </c>
       <c r="M649" s="5" t="s">
-        <v>8731</v>
+        <v>8730</v>
       </c>
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.4">
@@ -53919,7 +53931,7 @@
         <v>7071</v>
       </c>
       <c r="M650" s="5" t="s">
-        <v>8732</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="651" spans="1:13" x14ac:dyDescent="0.4">
@@ -53960,7 +53972,7 @@
         <v>7072</v>
       </c>
       <c r="M651" s="5" t="s">
-        <v>8733</v>
+        <v>8732</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.4">
@@ -54001,7 +54013,7 @@
         <v>7073</v>
       </c>
       <c r="M652" s="5" t="s">
-        <v>8734</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.4">
@@ -54042,7 +54054,7 @@
         <v>7074</v>
       </c>
       <c r="M653" s="5" t="s">
-        <v>8735</v>
+        <v>8734</v>
       </c>
     </row>
     <row r="654" spans="1:13" x14ac:dyDescent="0.4">
@@ -54083,7 +54095,7 @@
         <v>7075</v>
       </c>
       <c r="M654" s="5" t="s">
-        <v>8736</v>
+        <v>8735</v>
       </c>
     </row>
     <row r="655" spans="1:13" x14ac:dyDescent="0.4">
@@ -54124,7 +54136,7 @@
         <v>7076</v>
       </c>
       <c r="M655" s="5" t="s">
-        <v>8737</v>
+        <v>8736</v>
       </c>
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.4">
@@ -54165,7 +54177,7 @@
         <v>7077</v>
       </c>
       <c r="M656" s="5" t="s">
-        <v>8738</v>
+        <v>8737</v>
       </c>
     </row>
     <row r="657" spans="1:13" x14ac:dyDescent="0.4">
@@ -54206,7 +54218,7 @@
         <v>7078</v>
       </c>
       <c r="M657" s="5" t="s">
-        <v>8739</v>
+        <v>8738</v>
       </c>
     </row>
     <row r="658" spans="1:13" x14ac:dyDescent="0.4">
@@ -54247,7 +54259,7 @@
         <v>7079</v>
       </c>
       <c r="M658" s="5" t="s">
-        <v>8740</v>
+        <v>8739</v>
       </c>
     </row>
     <row r="659" spans="1:13" x14ac:dyDescent="0.4">
@@ -54288,7 +54300,7 @@
         <v>6492</v>
       </c>
       <c r="M659" s="5" t="s">
-        <v>8739</v>
+        <v>8738</v>
       </c>
     </row>
     <row r="660" spans="1:13" x14ac:dyDescent="0.4">
@@ -54329,7 +54341,7 @@
         <v>7080</v>
       </c>
       <c r="M660" s="5" t="s">
-        <v>8741</v>
+        <v>8740</v>
       </c>
     </row>
     <row r="661" spans="1:13" x14ac:dyDescent="0.4">
@@ -54370,7 +54382,7 @@
         <v>7081</v>
       </c>
       <c r="M661" s="5" t="s">
-        <v>8932</v>
+        <v>8931</v>
       </c>
     </row>
     <row r="662" spans="1:13" x14ac:dyDescent="0.4">
@@ -54411,7 +54423,7 @@
         <v>7116</v>
       </c>
       <c r="M662" s="5" t="s">
-        <v>8933</v>
+        <v>8932</v>
       </c>
     </row>
     <row r="663" spans="1:13" x14ac:dyDescent="0.4">
@@ -54452,7 +54464,7 @@
         <v>7082</v>
       </c>
       <c r="M663" s="5" t="s">
-        <v>8742</v>
+        <v>8741</v>
       </c>
     </row>
     <row r="664" spans="1:13" x14ac:dyDescent="0.4">
@@ -54493,7 +54505,7 @@
         <v>7083</v>
       </c>
       <c r="M664" s="5" t="s">
-        <v>8902</v>
+        <v>8901</v>
       </c>
     </row>
     <row r="665" spans="1:13" x14ac:dyDescent="0.4">
@@ -54534,7 +54546,7 @@
         <v>7084</v>
       </c>
       <c r="M665" s="5" t="s">
-        <v>8743</v>
+        <v>8742</v>
       </c>
     </row>
     <row r="666" spans="1:13" x14ac:dyDescent="0.4">
@@ -54575,7 +54587,7 @@
         <v>7085</v>
       </c>
       <c r="M666" s="5" t="s">
-        <v>8744</v>
+        <v>8743</v>
       </c>
     </row>
     <row r="667" spans="1:13" x14ac:dyDescent="0.4">
@@ -54616,7 +54628,7 @@
         <v>7086</v>
       </c>
       <c r="M667" s="5" t="s">
-        <v>8745</v>
+        <v>8744</v>
       </c>
     </row>
     <row r="668" spans="1:13" x14ac:dyDescent="0.4">
@@ -54657,7 +54669,7 @@
         <v>7087</v>
       </c>
       <c r="M668" s="5" t="s">
-        <v>8746</v>
+        <v>8745</v>
       </c>
     </row>
     <row r="669" spans="1:13" x14ac:dyDescent="0.4">
@@ -54698,7 +54710,7 @@
         <v>7088</v>
       </c>
       <c r="M669" s="5" t="s">
-        <v>8747</v>
+        <v>8746</v>
       </c>
     </row>
     <row r="670" spans="1:13" x14ac:dyDescent="0.4">
@@ -54739,7 +54751,7 @@
         <v>7089</v>
       </c>
       <c r="M670" s="5" t="s">
-        <v>8748</v>
+        <v>8747</v>
       </c>
     </row>
     <row r="671" spans="1:13" x14ac:dyDescent="0.4">
@@ -54780,7 +54792,7 @@
         <v>7090</v>
       </c>
       <c r="M671" s="5" t="s">
-        <v>8749</v>
+        <v>8748</v>
       </c>
     </row>
     <row r="672" spans="1:13" x14ac:dyDescent="0.4">
@@ -54821,7 +54833,7 @@
         <v>7091</v>
       </c>
       <c r="M672" s="5" t="s">
-        <v>8750</v>
+        <v>8749</v>
       </c>
     </row>
     <row r="673" spans="1:13" x14ac:dyDescent="0.4">
@@ -54862,7 +54874,7 @@
         <v>7092</v>
       </c>
       <c r="M673" s="5" t="s">
-        <v>8751</v>
+        <v>8750</v>
       </c>
     </row>
     <row r="674" spans="1:13" x14ac:dyDescent="0.4">
@@ -54903,7 +54915,7 @@
         <v>5876</v>
       </c>
       <c r="M674" s="5" t="s">
-        <v>8752</v>
+        <v>8751</v>
       </c>
     </row>
     <row r="675" spans="1:13" x14ac:dyDescent="0.4">
@@ -54944,7 +54956,7 @@
         <v>7053</v>
       </c>
       <c r="M675" s="5" t="s">
-        <v>8713</v>
+        <v>8712</v>
       </c>
     </row>
     <row r="676" spans="1:13" x14ac:dyDescent="0.4">
@@ -54985,7 +54997,7 @@
         <v>7093</v>
       </c>
       <c r="M676" s="5" t="s">
-        <v>8753</v>
+        <v>8752</v>
       </c>
     </row>
     <row r="677" spans="1:13" x14ac:dyDescent="0.4">
@@ -55026,7 +55038,7 @@
         <v>7094</v>
       </c>
       <c r="M677" s="5" t="s">
-        <v>8754</v>
+        <v>8753</v>
       </c>
     </row>
     <row r="678" spans="1:13" x14ac:dyDescent="0.4">
@@ -55067,7 +55079,7 @@
         <v>7095</v>
       </c>
       <c r="M678" s="5" t="s">
-        <v>8755</v>
+        <v>8754</v>
       </c>
     </row>
     <row r="679" spans="1:13" x14ac:dyDescent="0.4">
@@ -55108,7 +55120,7 @@
         <v>7096</v>
       </c>
       <c r="M679" s="5" t="s">
-        <v>8756</v>
+        <v>8755</v>
       </c>
     </row>
     <row r="680" spans="1:13" x14ac:dyDescent="0.4">
@@ -55149,7 +55161,7 @@
         <v>7097</v>
       </c>
       <c r="M680" s="5" t="s">
-        <v>8757</v>
+        <v>8756</v>
       </c>
     </row>
     <row r="681" spans="1:13" x14ac:dyDescent="0.4">
@@ -55190,7 +55202,7 @@
         <v>7098</v>
       </c>
       <c r="M681" s="5" t="s">
-        <v>8758</v>
+        <v>8757</v>
       </c>
     </row>
     <row r="682" spans="1:13" x14ac:dyDescent="0.4">
@@ -55231,7 +55243,7 @@
         <v>7099</v>
       </c>
       <c r="M682" s="5" t="s">
-        <v>8759</v>
+        <v>8758</v>
       </c>
     </row>
     <row r="683" spans="1:13" x14ac:dyDescent="0.4">
@@ -55272,7 +55284,7 @@
         <v>7100</v>
       </c>
       <c r="M683" s="5" t="s">
-        <v>8760</v>
+        <v>8759</v>
       </c>
     </row>
     <row r="684" spans="1:13" x14ac:dyDescent="0.4">
@@ -55313,7 +55325,7 @@
         <v>7101</v>
       </c>
       <c r="M684" s="5" t="s">
-        <v>8761</v>
+        <v>8760</v>
       </c>
     </row>
     <row r="685" spans="1:13" x14ac:dyDescent="0.4">
@@ -55354,7 +55366,7 @@
         <v>7102</v>
       </c>
       <c r="M685" s="5" t="s">
-        <v>8762</v>
+        <v>8761</v>
       </c>
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.4">
@@ -55395,7 +55407,7 @@
         <v>7103</v>
       </c>
       <c r="M686" s="5" t="s">
-        <v>8763</v>
+        <v>8762</v>
       </c>
     </row>
     <row r="687" spans="1:13" x14ac:dyDescent="0.4">
@@ -55436,7 +55448,7 @@
         <v>7104</v>
       </c>
       <c r="M687" s="5" t="s">
-        <v>8793</v>
+        <v>8792</v>
       </c>
     </row>
     <row r="688" spans="1:13" x14ac:dyDescent="0.4">
@@ -55477,7 +55489,7 @@
         <v>7105</v>
       </c>
       <c r="M688" s="5" t="s">
-        <v>8764</v>
+        <v>8763</v>
       </c>
     </row>
     <row r="689" spans="1:13" x14ac:dyDescent="0.4">
@@ -55518,7 +55530,7 @@
         <v>7106</v>
       </c>
       <c r="M689" s="5" t="s">
-        <v>8765</v>
+        <v>8764</v>
       </c>
     </row>
     <row r="690" spans="1:13" x14ac:dyDescent="0.4">
@@ -55559,7 +55571,7 @@
         <v>7107</v>
       </c>
       <c r="M690" s="5" t="s">
-        <v>8766</v>
+        <v>8765</v>
       </c>
     </row>
     <row r="691" spans="1:13" x14ac:dyDescent="0.4">
@@ -55600,7 +55612,7 @@
         <v>7108</v>
       </c>
       <c r="M691" s="5" t="s">
-        <v>8767</v>
+        <v>8766</v>
       </c>
     </row>
     <row r="692" spans="1:13" x14ac:dyDescent="0.4">
@@ -55641,7 +55653,7 @@
         <v>7109</v>
       </c>
       <c r="M692" s="5" t="s">
-        <v>8768</v>
+        <v>8767</v>
       </c>
     </row>
     <row r="693" spans="1:13" x14ac:dyDescent="0.4">
@@ -55682,7 +55694,7 @@
         <v>7133</v>
       </c>
       <c r="M693" s="5" t="s">
-        <v>8903</v>
+        <v>8902</v>
       </c>
     </row>
     <row r="694" spans="1:13" x14ac:dyDescent="0.4">
@@ -55723,7 +55735,7 @@
         <v>7136</v>
       </c>
       <c r="M694" s="5" t="s">
-        <v>8769</v>
+        <v>8768</v>
       </c>
     </row>
     <row r="695" spans="1:13" x14ac:dyDescent="0.4">
@@ -55764,7 +55776,7 @@
         <v>7155</v>
       </c>
       <c r="M695" s="5" t="s">
-        <v>8794</v>
+        <v>8793</v>
       </c>
     </row>
     <row r="696" spans="1:13" x14ac:dyDescent="0.4">
@@ -55805,7 +55817,7 @@
         <v>7849</v>
       </c>
       <c r="M696" s="5" t="s">
-        <v>8770</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="697" spans="1:13" x14ac:dyDescent="0.4">
@@ -55846,7 +55858,7 @@
         <v>7948</v>
       </c>
       <c r="M697" s="5" t="s">
-        <v>8771</v>
+        <v>8770</v>
       </c>
     </row>
     <row r="698" spans="1:13" x14ac:dyDescent="0.4">
@@ -55887,7 +55899,7 @@
         <v>7949</v>
       </c>
       <c r="M698" s="5" t="s">
-        <v>8772</v>
+        <v>8771</v>
       </c>
     </row>
     <row r="699" spans="1:13" x14ac:dyDescent="0.4">
@@ -55928,7 +55940,7 @@
         <v>8030</v>
       </c>
       <c r="M699" s="5" t="s">
-        <v>8773</v>
+        <v>8772</v>
       </c>
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.4">
@@ -55969,7 +55981,7 @@
         <v>8052</v>
       </c>
       <c r="M700" s="5" t="s">
-        <v>8774</v>
+        <v>8773</v>
       </c>
     </row>
     <row r="701" spans="1:13" x14ac:dyDescent="0.4">
@@ -56010,7 +56022,7 @@
         <v>8053</v>
       </c>
       <c r="M701" s="5" t="s">
-        <v>8775</v>
+        <v>8774</v>
       </c>
     </row>
     <row r="702" spans="1:13" x14ac:dyDescent="0.4">
@@ -56051,7 +56063,7 @@
         <v>8063</v>
       </c>
       <c r="M702" s="5" t="s">
-        <v>8776</v>
+        <v>8775</v>
       </c>
     </row>
     <row r="703" spans="1:13" x14ac:dyDescent="0.4">
@@ -56092,7 +56104,7 @@
         <v>8064</v>
       </c>
       <c r="M703" s="5" t="s">
-        <v>8904</v>
+        <v>8903</v>
       </c>
     </row>
     <row r="704" spans="1:13" x14ac:dyDescent="0.4">
@@ -56133,7 +56145,7 @@
         <v>8065</v>
       </c>
       <c r="M704" s="5" t="s">
-        <v>8777</v>
+        <v>8776</v>
       </c>
     </row>
     <row r="705" spans="1:13" x14ac:dyDescent="0.4">
@@ -56174,7 +56186,7 @@
         <v>8107</v>
       </c>
       <c r="M705" s="5" t="s">
-        <v>8795</v>
+        <v>8794</v>
       </c>
     </row>
     <row r="706" spans="1:13" x14ac:dyDescent="0.4">
@@ -56215,7 +56227,7 @@
         <v>8123</v>
       </c>
       <c r="M706" s="5" t="s">
-        <v>8796</v>
+        <v>8795</v>
       </c>
     </row>
     <row r="707" spans="1:13" x14ac:dyDescent="0.4">
@@ -56256,7 +56268,7 @@
         <v>8133</v>
       </c>
       <c r="M707" s="5" t="s">
-        <v>8797</v>
+        <v>8796</v>
       </c>
     </row>
     <row r="708" spans="1:13" x14ac:dyDescent="0.4">
@@ -56297,7 +56309,7 @@
         <v>8146</v>
       </c>
       <c r="M708" s="5" t="s">
-        <v>8798</v>
+        <v>8797</v>
       </c>
     </row>
     <row r="709" spans="1:13" x14ac:dyDescent="0.4">
@@ -56338,7 +56350,7 @@
         <v>8165</v>
       </c>
       <c r="M709" s="5" t="s">
-        <v>8905</v>
+        <v>8904</v>
       </c>
     </row>
     <row r="710" spans="1:13" x14ac:dyDescent="0.4">
@@ -56379,7 +56391,7 @@
         <v>8145</v>
       </c>
       <c r="M710" s="5" t="s">
-        <v>8778</v>
+        <v>8777</v>
       </c>
     </row>
     <row r="711" spans="1:13" x14ac:dyDescent="0.4">
@@ -56420,7 +56432,7 @@
         <v>8186</v>
       </c>
       <c r="M711" s="5" t="s">
-        <v>8779</v>
+        <v>8778</v>
       </c>
     </row>
     <row r="712" spans="1:13" x14ac:dyDescent="0.4">
@@ -56461,7 +56473,7 @@
         <v>8187</v>
       </c>
       <c r="M712" s="5" t="s">
-        <v>8780</v>
+        <v>8779</v>
       </c>
     </row>
     <row r="713" spans="1:13" x14ac:dyDescent="0.4">
@@ -56502,7 +56514,7 @@
         <v>8188</v>
       </c>
       <c r="M713" s="5" t="s">
-        <v>8781</v>
+        <v>8780</v>
       </c>
     </row>
     <row r="714" spans="1:13" x14ac:dyDescent="0.4">
@@ -56543,11 +56555,11 @@
         <v>8189</v>
       </c>
       <c r="M714" s="5" t="s">
-        <v>8782</v>
+        <v>8781</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>